<commit_message>
Truncate all measurements to integers in fake_data.xlsx
Round temperature, Variable_1, Variable_2 to integers in both
the Excel file and the HTML preview table.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/fake_data.xlsx
+++ b/fake_data.xlsx
@@ -16,9 +16,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -52,10 +51,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -458,1403 +458,1403 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n">
+      <c r="A2" s="3" t="n">
         <v>45658</v>
       </c>
       <c r="B2" t="n">
         <v>13</v>
       </c>
       <c r="C2" t="n">
-        <v>71.69</v>
+        <v>71</v>
       </c>
       <c r="D2" t="n">
-        <v>92.04000000000001</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="n">
+      <c r="A3" s="3" t="n">
         <v>45659</v>
       </c>
       <c r="B3" t="n">
         <v>10</v>
       </c>
       <c r="C3" t="n">
-        <v>91.59</v>
+        <v>91</v>
       </c>
       <c r="D3" t="n">
-        <v>105.51</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="n">
+      <c r="A4" s="3" t="n">
         <v>45660</v>
       </c>
       <c r="B4" t="n">
         <v>14</v>
       </c>
       <c r="C4" t="n">
-        <v>93.15000000000001</v>
+        <v>93</v>
       </c>
       <c r="D4" t="n">
-        <v>115.33</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="n">
+      <c r="A5" s="3" t="n">
         <v>45661</v>
       </c>
       <c r="B5" t="n">
-        <v>18.5</v>
+        <v>18</v>
       </c>
       <c r="C5" t="n">
-        <v>83.95</v>
+        <v>83</v>
       </c>
       <c r="D5" t="n">
-        <v>110.23</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="n">
+      <c r="A6" s="3" t="n">
         <v>45662</v>
       </c>
       <c r="B6" t="n">
-        <v>9.800000000000001</v>
+        <v>9</v>
       </c>
       <c r="C6" t="n">
-        <v>96.77</v>
+        <v>96</v>
       </c>
       <c r="D6" t="n">
-        <v>74.53</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="n">
+      <c r="A7" s="3" t="n">
         <v>45663</v>
       </c>
       <c r="B7" t="n">
-        <v>9.9</v>
+        <v>9</v>
       </c>
       <c r="C7" t="n">
-        <v>108.08</v>
+        <v>108</v>
       </c>
       <c r="D7" t="n">
-        <v>87.8</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="n">
+      <c r="A8" s="3" t="n">
         <v>45664</v>
       </c>
       <c r="B8" t="n">
-        <v>19.1</v>
+        <v>19</v>
       </c>
       <c r="C8" t="n">
-        <v>137.72</v>
+        <v>137</v>
       </c>
       <c r="D8" t="n">
-        <v>127.78</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="n">
+      <c r="A9" s="3" t="n">
         <v>45665</v>
       </c>
       <c r="B9" t="n">
-        <v>15.2</v>
+        <v>15</v>
       </c>
       <c r="C9" t="n">
-        <v>103.49</v>
+        <v>103</v>
       </c>
       <c r="D9" t="n">
-        <v>110.64</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="n">
+      <c r="A10" s="3" t="n">
         <v>45666</v>
       </c>
       <c r="B10" t="n">
-        <v>9.199999999999999</v>
+        <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>105.15</v>
+        <v>105</v>
       </c>
       <c r="D10" t="n">
-        <v>111.5</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="n">
+      <c r="A11" s="3" t="n">
         <v>45667</v>
       </c>
       <c r="B11" t="n">
-        <v>14.4</v>
+        <v>14</v>
       </c>
       <c r="C11" t="n">
-        <v>98.51000000000001</v>
+        <v>98</v>
       </c>
       <c r="D11" t="n">
-        <v>165.99</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="n">
+      <c r="A12" s="3" t="n">
         <v>45668</v>
       </c>
       <c r="B12" t="n">
-        <v>9.5</v>
+        <v>9</v>
       </c>
       <c r="C12" t="n">
-        <v>61.62</v>
+        <v>61</v>
       </c>
       <c r="D12" t="n">
-        <v>90.7</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="n">
+      <c r="A13" s="3" t="n">
         <v>45669</v>
       </c>
       <c r="B13" t="n">
-        <v>9.6</v>
+        <v>9</v>
       </c>
       <c r="C13" t="n">
-        <v>99.47</v>
+        <v>99</v>
       </c>
       <c r="D13" t="n">
-        <v>119.4</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="n">
+      <c r="A14" s="3" t="n">
         <v>45670</v>
       </c>
       <c r="B14" t="n">
-        <v>13.4</v>
+        <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>101.2</v>
+        <v>101</v>
       </c>
       <c r="D14" t="n">
-        <v>117.13</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="n">
+      <c r="A15" s="3" t="n">
         <v>45671</v>
       </c>
       <c r="B15" t="n">
-        <v>2.8</v>
+        <v>2</v>
       </c>
       <c r="C15" t="n">
-        <v>149.26</v>
+        <v>149</v>
       </c>
       <c r="D15" t="n">
-        <v>135.91</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="2" t="n">
+      <c r="A16" s="3" t="n">
         <v>45672</v>
       </c>
       <c r="B16" t="n">
-        <v>3.9</v>
+        <v>3</v>
       </c>
       <c r="C16" t="n">
-        <v>96.15000000000001</v>
+        <v>96</v>
       </c>
       <c r="D16" t="n">
-        <v>92.62</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="2" t="n">
+      <c r="A17" s="3" t="n">
         <v>45673</v>
       </c>
       <c r="B17" t="n">
-        <v>9.9</v>
+        <v>9</v>
       </c>
       <c r="C17" t="n">
-        <v>106.03</v>
+        <v>106</v>
       </c>
       <c r="D17" t="n">
-        <v>116.16</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="2" t="n">
+      <c r="A18" s="3" t="n">
         <v>45674</v>
       </c>
       <c r="B18" t="n">
-        <v>7.8</v>
+        <v>7</v>
       </c>
       <c r="C18" t="n">
-        <v>99.31</v>
+        <v>99</v>
       </c>
       <c r="D18" t="n">
-        <v>86.27</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="2" t="n">
+      <c r="A19" s="3" t="n">
         <v>45675</v>
       </c>
       <c r="B19" t="n">
-        <v>14.7</v>
+        <v>14</v>
       </c>
       <c r="C19" t="n">
-        <v>76.63</v>
+        <v>76</v>
       </c>
       <c r="D19" t="n">
-        <v>84.20999999999999</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="2" t="n">
+      <c r="A20" s="3" t="n">
         <v>45676</v>
       </c>
       <c r="B20" t="n">
-        <v>8.800000000000001</v>
+        <v>8</v>
       </c>
       <c r="C20" t="n">
-        <v>122.86</v>
+        <v>122</v>
       </c>
       <c r="D20" t="n">
-        <v>103.02</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="2" t="n">
+      <c r="A21" s="3" t="n">
         <v>45677</v>
       </c>
       <c r="B21" t="n">
-        <v>6.5</v>
+        <v>6</v>
       </c>
       <c r="C21" t="n">
-        <v>115.04</v>
+        <v>115</v>
       </c>
       <c r="D21" t="n">
-        <v>108.94</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="2" t="n">
+      <c r="A22" s="3" t="n">
         <v>45678</v>
       </c>
       <c r="B22" t="n">
-        <v>21.1</v>
+        <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>115.82</v>
+        <v>115</v>
       </c>
       <c r="D22" t="n">
         <v>148</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="2" t="n">
+      <c r="A23" s="3" t="n">
         <v>45679</v>
       </c>
       <c r="B23" t="n">
-        <v>12.9</v>
+        <v>12</v>
       </c>
       <c r="C23" t="n">
-        <v>81.81</v>
+        <v>81</v>
       </c>
       <c r="D23" t="n">
-        <v>58.56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="2" t="n">
+      <c r="A24" s="3" t="n">
         <v>45680</v>
       </c>
       <c r="B24" t="n">
-        <v>14.6</v>
+        <v>14</v>
       </c>
       <c r="C24" t="n">
-        <v>128.06</v>
+        <v>128</v>
       </c>
       <c r="D24" t="n">
-        <v>125.91</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="2" t="n">
+      <c r="A25" s="3" t="n">
         <v>45681</v>
       </c>
       <c r="B25" t="n">
-        <v>7.3</v>
+        <v>7</v>
       </c>
       <c r="C25" t="n">
-        <v>71.95999999999999</v>
+        <v>71</v>
       </c>
       <c r="D25" t="n">
-        <v>58.05</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="2" t="n">
+      <c r="A26" s="3" t="n">
         <v>45682</v>
       </c>
       <c r="B26" t="n">
         <v>12</v>
       </c>
       <c r="C26" t="n">
-        <v>111.74</v>
+        <v>111</v>
       </c>
       <c r="D26" t="n">
-        <v>97.69</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="2" t="n">
+      <c r="A27" s="3" t="n">
         <v>45683</v>
       </c>
       <c r="B27" t="n">
-        <v>15.5</v>
+        <v>15</v>
       </c>
       <c r="C27" t="n">
-        <v>143.81</v>
+        <v>143</v>
       </c>
       <c r="D27" t="n">
-        <v>140.77</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="2" t="n">
+      <c r="A28" s="3" t="n">
         <v>45684</v>
       </c>
       <c r="B28" t="n">
-        <v>9.5</v>
+        <v>9</v>
       </c>
       <c r="C28" t="n">
-        <v>80.19</v>
+        <v>80</v>
       </c>
       <c r="D28" t="n">
-        <v>91.20999999999999</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="2" t="n">
+      <c r="A29" s="3" t="n">
         <v>45685</v>
       </c>
       <c r="B29" t="n">
-        <v>17.4</v>
+        <v>17</v>
       </c>
       <c r="C29" t="n">
-        <v>88.67</v>
+        <v>88</v>
       </c>
       <c r="D29" t="n">
-        <v>75.67</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="2" t="n">
+      <c r="A30" s="3" t="n">
         <v>45686</v>
       </c>
       <c r="B30" t="n">
-        <v>12.8</v>
+        <v>12</v>
       </c>
       <c r="C30" t="n">
-        <v>101.99</v>
+        <v>101</v>
       </c>
       <c r="D30" t="n">
-        <v>88.61</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="2" t="n">
+      <c r="A31" s="3" t="n">
         <v>45687</v>
       </c>
       <c r="B31" t="n">
-        <v>14.6</v>
+        <v>14</v>
       </c>
       <c r="C31" t="n">
-        <v>89.93000000000001</v>
+        <v>89</v>
       </c>
       <c r="D31" t="n">
-        <v>106.74</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="2" t="n">
+      <c r="A32" s="3" t="n">
         <v>45688</v>
       </c>
       <c r="B32" t="n">
-        <v>13.3</v>
+        <v>13</v>
       </c>
       <c r="C32" t="n">
-        <v>68.98999999999999</v>
+        <v>68</v>
       </c>
       <c r="D32" t="n">
-        <v>71.84</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="2" t="n">
+      <c r="A33" s="3" t="n">
         <v>45689</v>
       </c>
       <c r="B33" t="n">
-        <v>25.9</v>
+        <v>25</v>
       </c>
       <c r="C33" t="n">
-        <v>101.37</v>
+        <v>101</v>
       </c>
       <c r="D33" t="n">
-        <v>104.43</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="2" t="n">
+      <c r="A34" s="3" t="n">
         <v>45690</v>
       </c>
       <c r="B34" t="n">
-        <v>16.8</v>
+        <v>16</v>
       </c>
       <c r="C34" t="n">
-        <v>78.75</v>
+        <v>78</v>
       </c>
       <c r="D34" t="n">
-        <v>90.17</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="2" t="n">
+      <c r="A35" s="3" t="n">
         <v>45691</v>
       </c>
       <c r="B35" t="n">
-        <v>11.9</v>
+        <v>11</v>
       </c>
       <c r="C35" t="n">
-        <v>109.47</v>
+        <v>109</v>
       </c>
       <c r="D35" t="n">
-        <v>93.45</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="2" t="n">
+      <c r="A36" s="3" t="n">
         <v>45692</v>
       </c>
       <c r="B36" t="n">
-        <v>21.6</v>
+        <v>21</v>
       </c>
       <c r="C36" t="n">
-        <v>81.61</v>
+        <v>81</v>
       </c>
       <c r="D36" t="n">
-        <v>127.94</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="2" t="n">
+      <c r="A37" s="3" t="n">
         <v>45693</v>
       </c>
       <c r="B37" t="n">
-        <v>11.7</v>
+        <v>11</v>
       </c>
       <c r="C37" t="n">
         <v>131</v>
       </c>
       <c r="D37" t="n">
-        <v>126.48</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="2" t="n">
+      <c r="A38" s="3" t="n">
         <v>45694</v>
       </c>
       <c r="B38" t="n">
-        <v>19.2</v>
+        <v>19</v>
       </c>
       <c r="C38" t="n">
-        <v>84.33</v>
+        <v>84</v>
       </c>
       <c r="D38" t="n">
-        <v>57.09</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="2" t="n">
+      <c r="A39" s="3" t="n">
         <v>45695</v>
       </c>
       <c r="B39" t="n">
-        <v>8.699999999999999</v>
+        <v>8</v>
       </c>
       <c r="C39" t="n">
-        <v>93.56</v>
+        <v>93</v>
       </c>
       <c r="D39" t="n">
-        <v>100.01</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="2" t="n">
+      <c r="A40" s="3" t="n">
         <v>45696</v>
       </c>
       <c r="B40" t="n">
-        <v>12.1</v>
+        <v>12</v>
       </c>
       <c r="C40" t="n">
-        <v>116.27</v>
+        <v>116</v>
       </c>
       <c r="D40" t="n">
-        <v>96.67</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="2" t="n">
+      <c r="A41" s="3" t="n">
         <v>45697</v>
       </c>
       <c r="B41" t="n">
-        <v>20.1</v>
+        <v>20</v>
       </c>
       <c r="C41" t="n">
-        <v>75.38</v>
+        <v>75</v>
       </c>
       <c r="D41" t="n">
-        <v>102.46</v>
+        <v>102</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="2" t="n">
+      <c r="A42" s="3" t="n">
         <v>45698</v>
       </c>
       <c r="B42" t="n">
-        <v>23.1</v>
+        <v>23</v>
       </c>
       <c r="C42" t="n">
-        <v>104.55</v>
+        <v>104</v>
       </c>
       <c r="D42" t="n">
-        <v>88.55</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="2" t="n">
+      <c r="A43" s="3" t="n">
         <v>45699</v>
       </c>
       <c r="B43" t="n">
-        <v>20.6</v>
+        <v>20</v>
       </c>
       <c r="C43" t="n">
-        <v>126.14</v>
+        <v>126</v>
       </c>
       <c r="D43" t="n">
-        <v>111.08</v>
+        <v>111</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="2" t="n">
+      <c r="A44" s="3" t="n">
         <v>45700</v>
       </c>
       <c r="B44" t="n">
-        <v>19.6</v>
+        <v>19</v>
       </c>
       <c r="C44" t="n">
-        <v>67.84999999999999</v>
+        <v>67</v>
       </c>
       <c r="D44" t="n">
-        <v>92.67</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="2" t="n">
+      <c r="A45" s="3" t="n">
         <v>45701</v>
       </c>
       <c r="B45" t="n">
         <v>19</v>
       </c>
       <c r="C45" t="n">
-        <v>103.69</v>
+        <v>103</v>
       </c>
       <c r="D45" t="n">
-        <v>116.84</v>
+        <v>116</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="2" t="n">
+      <c r="A46" s="3" t="n">
         <v>45702</v>
       </c>
       <c r="B46" t="n">
-        <v>13.4</v>
+        <v>13</v>
       </c>
       <c r="C46" t="n">
-        <v>105.2</v>
+        <v>105</v>
       </c>
       <c r="D46" t="n">
-        <v>81.81</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="2" t="n">
+      <c r="A47" s="3" t="n">
         <v>45703</v>
       </c>
       <c r="B47" t="n">
-        <v>17.6</v>
+        <v>17</v>
       </c>
       <c r="C47" t="n">
-        <v>115.64</v>
+        <v>115</v>
       </c>
       <c r="D47" t="n">
-        <v>102.02</v>
+        <v>102</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="2" t="n">
+      <c r="A48" s="3" t="n">
         <v>45704</v>
       </c>
       <c r="B48" t="n">
-        <v>19.2</v>
+        <v>19</v>
       </c>
       <c r="C48" t="n">
-        <v>75.26000000000001</v>
+        <v>75</v>
       </c>
       <c r="D48" t="n">
-        <v>79.40000000000001</v>
+        <v>79</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="2" t="n">
+      <c r="A49" s="3" t="n">
         <v>45705</v>
       </c>
       <c r="B49" t="n">
-        <v>27.2</v>
+        <v>27</v>
       </c>
       <c r="C49" t="n">
-        <v>73.59</v>
+        <v>73</v>
       </c>
       <c r="D49" t="n">
-        <v>75.48</v>
+        <v>75</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="2" t="n">
+      <c r="A50" s="3" t="n">
         <v>45706</v>
       </c>
       <c r="B50" t="n">
         <v>24</v>
       </c>
       <c r="C50" t="n">
-        <v>110.44</v>
+        <v>110</v>
       </c>
       <c r="D50" t="n">
-        <v>135.8</v>
+        <v>135</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="2" t="n">
+      <c r="A51" s="3" t="n">
         <v>45707</v>
       </c>
       <c r="B51" t="n">
-        <v>13.8</v>
+        <v>13</v>
       </c>
       <c r="C51" t="n">
-        <v>105.94</v>
+        <v>105</v>
       </c>
       <c r="D51" t="n">
-        <v>109.98</v>
+        <v>109</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="2" t="n">
+      <c r="A52" s="3" t="n">
         <v>45708</v>
       </c>
       <c r="B52" t="n">
-        <v>24.7</v>
+        <v>24</v>
       </c>
       <c r="C52" t="n">
-        <v>105.01</v>
+        <v>105</v>
       </c>
       <c r="D52" t="n">
-        <v>80.67</v>
+        <v>80</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="2" t="n">
+      <c r="A53" s="3" t="n">
         <v>45709</v>
       </c>
       <c r="B53" t="n">
-        <v>21.5</v>
+        <v>21</v>
       </c>
       <c r="C53" t="n">
-        <v>106.93</v>
+        <v>106</v>
       </c>
       <c r="D53" t="n">
-        <v>119.36</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="2" t="n">
+      <c r="A54" s="3" t="n">
         <v>45710</v>
       </c>
       <c r="B54" t="n">
-        <v>20.4</v>
+        <v>20</v>
       </c>
       <c r="C54" t="n">
-        <v>86.40000000000001</v>
+        <v>86</v>
       </c>
       <c r="D54" t="n">
-        <v>129.96</v>
+        <v>129</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="2" t="n">
+      <c r="A55" s="3" t="n">
         <v>45711</v>
       </c>
       <c r="B55" t="n">
-        <v>27.2</v>
+        <v>27</v>
       </c>
       <c r="C55" t="n">
-        <v>104.65</v>
+        <v>104</v>
       </c>
       <c r="D55" t="n">
-        <v>120.21</v>
+        <v>120</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="2" t="n">
+      <c r="A56" s="3" t="n">
         <v>45712</v>
       </c>
       <c r="B56" t="n">
-        <v>29.7</v>
+        <v>29</v>
       </c>
       <c r="C56" t="n">
-        <v>105.86</v>
+        <v>105</v>
       </c>
       <c r="D56" t="n">
-        <v>76.61</v>
+        <v>76</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="2" t="n">
+      <c r="A57" s="3" t="n">
         <v>45713</v>
       </c>
       <c r="B57" t="n">
-        <v>29.6</v>
+        <v>29</v>
       </c>
       <c r="C57" t="n">
-        <v>85.70999999999999</v>
+        <v>85</v>
       </c>
       <c r="D57" t="n">
-        <v>84.47</v>
+        <v>84</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="2" t="n">
+      <c r="A58" s="3" t="n">
         <v>45714</v>
       </c>
       <c r="B58" t="n">
-        <v>21.2</v>
+        <v>21</v>
       </c>
       <c r="C58" t="n">
-        <v>137.32</v>
+        <v>137</v>
       </c>
       <c r="D58" t="n">
-        <v>140.6</v>
+        <v>140</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="2" t="n">
+      <c r="A59" s="3" t="n">
         <v>45715</v>
       </c>
       <c r="B59" t="n">
-        <v>24.2</v>
+        <v>24</v>
       </c>
       <c r="C59" t="n">
-        <v>109.48</v>
+        <v>109</v>
       </c>
       <c r="D59" t="n">
-        <v>92.48</v>
+        <v>92</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="2" t="n">
+      <c r="A60" s="3" t="n">
         <v>45716</v>
       </c>
       <c r="B60" t="n">
-        <v>27.8</v>
+        <v>27</v>
       </c>
       <c r="C60" t="n">
-        <v>76.17</v>
+        <v>76</v>
       </c>
       <c r="D60" t="n">
-        <v>95.77</v>
+        <v>95</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="2" t="n">
+      <c r="A61" s="3" t="n">
         <v>45717</v>
       </c>
       <c r="B61" t="n">
-        <v>31.4</v>
+        <v>31</v>
       </c>
       <c r="C61" t="n">
-        <v>113.13</v>
+        <v>113</v>
       </c>
       <c r="D61" t="n">
-        <v>119.98</v>
+        <v>119</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="2" t="n">
+      <c r="A62" s="3" t="n">
         <v>45718</v>
       </c>
       <c r="B62" t="n">
-        <v>24.6</v>
+        <v>24</v>
       </c>
       <c r="C62" t="n">
-        <v>80.51000000000001</v>
+        <v>80</v>
       </c>
       <c r="D62" t="n">
-        <v>74.2</v>
+        <v>74</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="2" t="n">
+      <c r="A63" s="3" t="n">
         <v>45719</v>
       </c>
       <c r="B63" t="n">
-        <v>26.4</v>
+        <v>26</v>
       </c>
       <c r="C63" t="n">
-        <v>115.74</v>
+        <v>115</v>
       </c>
       <c r="D63" t="n">
-        <v>106.84</v>
+        <v>106</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="2" t="n">
+      <c r="A64" s="3" t="n">
         <v>45720</v>
       </c>
       <c r="B64" t="n">
-        <v>22.3</v>
+        <v>22</v>
       </c>
       <c r="C64" t="n">
-        <v>123.17</v>
+        <v>123</v>
       </c>
       <c r="D64" t="n">
-        <v>55.45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="2" t="n">
+      <c r="A65" s="3" t="n">
         <v>45721</v>
       </c>
       <c r="B65" t="n">
-        <v>22.2</v>
+        <v>22</v>
       </c>
       <c r="C65" t="n">
-        <v>83.59</v>
+        <v>83</v>
       </c>
       <c r="D65" t="n">
-        <v>74.05</v>
+        <v>74</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="2" t="n">
+      <c r="A66" s="3" t="n">
         <v>45722</v>
       </c>
       <c r="B66" t="n">
-        <v>32.7</v>
+        <v>32</v>
       </c>
       <c r="C66" t="n">
-        <v>119.27</v>
+        <v>119</v>
       </c>
       <c r="D66" t="n">
-        <v>105.26</v>
+        <v>105</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="2" t="n">
+      <c r="A67" s="3" t="n">
         <v>45723</v>
       </c>
       <c r="B67" t="n">
-        <v>35.8</v>
+        <v>35</v>
       </c>
       <c r="C67" t="n">
-        <v>108.26</v>
+        <v>108</v>
       </c>
       <c r="D67" t="n">
-        <v>82.52</v>
+        <v>82</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="2" t="n">
+      <c r="A68" s="3" t="n">
         <v>45724</v>
       </c>
       <c r="B68" t="n">
-        <v>29.1</v>
+        <v>29</v>
       </c>
       <c r="C68" t="n">
-        <v>116.44</v>
+        <v>116</v>
       </c>
       <c r="D68" t="n">
-        <v>136.49</v>
+        <v>136</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="2" t="n">
+      <c r="A69" s="3" t="n">
         <v>45725</v>
       </c>
       <c r="B69" t="n">
-        <v>34.9</v>
+        <v>34</v>
       </c>
       <c r="C69" t="n">
-        <v>137.94</v>
+        <v>137</v>
       </c>
       <c r="D69" t="n">
-        <v>94.2</v>
+        <v>94</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="2" t="n">
+      <c r="A70" s="3" t="n">
         <v>45726</v>
       </c>
       <c r="B70" t="n">
-        <v>32.1</v>
+        <v>32</v>
       </c>
       <c r="C70" t="n">
-        <v>95.09</v>
+        <v>95</v>
       </c>
       <c r="D70" t="n">
-        <v>89.92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="2" t="n">
+      <c r="A71" s="3" t="n">
         <v>45727</v>
       </c>
       <c r="B71" t="n">
-        <v>27.5</v>
+        <v>27</v>
       </c>
       <c r="C71" t="n">
-        <v>84.93000000000001</v>
+        <v>84</v>
       </c>
       <c r="D71" t="n">
-        <v>94.73</v>
+        <v>94</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="2" t="n">
+      <c r="A72" s="3" t="n">
         <v>45728</v>
       </c>
       <c r="B72" t="n">
-        <v>32.9</v>
+        <v>32</v>
       </c>
       <c r="C72" t="n">
-        <v>82.20999999999999</v>
+        <v>82</v>
       </c>
       <c r="D72" t="n">
-        <v>116.07</v>
+        <v>116</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="2" t="n">
+      <c r="A73" s="3" t="n">
         <v>45729</v>
       </c>
       <c r="B73" t="n">
-        <v>39.3</v>
+        <v>39</v>
       </c>
       <c r="C73" t="n">
-        <v>83.68000000000001</v>
+        <v>83</v>
       </c>
       <c r="D73" t="n">
-        <v>66.97</v>
+        <v>66</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="2" t="n">
+      <c r="A74" s="3" t="n">
         <v>45730</v>
       </c>
       <c r="B74" t="n">
-        <v>31.8</v>
+        <v>31</v>
       </c>
       <c r="C74" t="n">
-        <v>98.45999999999999</v>
+        <v>98</v>
       </c>
       <c r="D74" t="n">
-        <v>119.38</v>
+        <v>119</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="2" t="n">
+      <c r="A75" s="3" t="n">
         <v>45731</v>
       </c>
       <c r="B75" t="n">
-        <v>40.2</v>
+        <v>40</v>
       </c>
       <c r="C75" t="n">
-        <v>106.82</v>
+        <v>106</v>
       </c>
       <c r="D75" t="n">
-        <v>103.59</v>
+        <v>103</v>
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="2" t="n">
+      <c r="A76" s="3" t="n">
         <v>45732</v>
       </c>
       <c r="B76" t="n">
-        <v>19.8</v>
+        <v>19</v>
       </c>
       <c r="C76" t="n">
-        <v>105.53</v>
+        <v>105</v>
       </c>
       <c r="D76" t="n">
-        <v>85.77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="2" t="n">
+      <c r="A77" s="3" t="n">
         <v>45733</v>
       </c>
       <c r="B77" t="n">
-        <v>37.4</v>
+        <v>37</v>
       </c>
       <c r="C77" t="n">
-        <v>116.54</v>
+        <v>116</v>
       </c>
       <c r="D77" t="n">
-        <v>116.28</v>
+        <v>116</v>
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="2" t="n">
+      <c r="A78" s="3" t="n">
         <v>45734</v>
       </c>
       <c r="B78" t="n">
-        <v>34.1</v>
+        <v>34</v>
       </c>
       <c r="C78" t="n">
-        <v>100.26</v>
+        <v>100</v>
       </c>
       <c r="D78" t="n">
-        <v>103.58</v>
+        <v>103</v>
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="2" t="n">
+      <c r="A79" s="3" t="n">
         <v>45735</v>
       </c>
       <c r="B79" t="n">
-        <v>32.6</v>
+        <v>32</v>
       </c>
       <c r="C79" t="n">
-        <v>129.07</v>
+        <v>129</v>
       </c>
       <c r="D79" t="n">
-        <v>104.14</v>
+        <v>104</v>
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="2" t="n">
+      <c r="A80" s="3" t="n">
         <v>45736</v>
       </c>
       <c r="B80" t="n">
         <v>35</v>
       </c>
       <c r="C80" t="n">
-        <v>94.70999999999999</v>
+        <v>94</v>
       </c>
       <c r="D80" t="n">
-        <v>98.56</v>
+        <v>98</v>
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="2" t="n">
+      <c r="A81" s="3" t="n">
         <v>45737</v>
       </c>
       <c r="B81" t="n">
-        <v>25.1</v>
+        <v>25</v>
       </c>
       <c r="C81" t="n">
-        <v>154.4</v>
+        <v>154</v>
       </c>
       <c r="D81" t="n">
-        <v>120.53</v>
+        <v>120</v>
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="2" t="n">
+      <c r="A82" s="3" t="n">
         <v>45738</v>
       </c>
       <c r="B82" t="n">
-        <v>34.3</v>
+        <v>34</v>
       </c>
       <c r="C82" t="n">
-        <v>112.51</v>
+        <v>112</v>
       </c>
       <c r="D82" t="n">
-        <v>108.22</v>
+        <v>108</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="2" t="n">
+      <c r="A83" s="3" t="n">
         <v>45739</v>
       </c>
       <c r="B83" t="n">
-        <v>37.6</v>
+        <v>37</v>
       </c>
       <c r="C83" t="n">
-        <v>82.86</v>
+        <v>82</v>
       </c>
       <c r="D83" t="n">
-        <v>102.9</v>
+        <v>102</v>
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="2" t="n">
+      <c r="A84" s="3" t="n">
         <v>45740</v>
       </c>
       <c r="B84" t="n">
-        <v>43.7</v>
+        <v>43</v>
       </c>
       <c r="C84" t="n">
-        <v>78.58</v>
+        <v>78</v>
       </c>
       <c r="D84" t="n">
-        <v>116.76</v>
+        <v>116</v>
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="2" t="n">
+      <c r="A85" s="3" t="n">
         <v>45741</v>
       </c>
       <c r="B85" t="n">
-        <v>34.1</v>
+        <v>34</v>
       </c>
       <c r="C85" t="n">
-        <v>109.65</v>
+        <v>109</v>
       </c>
       <c r="D85" t="n">
-        <v>83.39</v>
+        <v>83</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="2" t="n">
+      <c r="A86" s="3" t="n">
         <v>45742</v>
       </c>
       <c r="B86" t="n">
-        <v>33.1</v>
+        <v>33</v>
       </c>
       <c r="C86" t="n">
-        <v>95.53</v>
+        <v>95</v>
       </c>
       <c r="D86" t="n">
-        <v>134.71</v>
+        <v>134</v>
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="2" t="n">
+      <c r="A87" s="3" t="n">
         <v>45743</v>
       </c>
       <c r="B87" t="n">
-        <v>35.1</v>
+        <v>35</v>
       </c>
       <c r="C87" t="n">
-        <v>114.28</v>
+        <v>114</v>
       </c>
       <c r="D87" t="n">
-        <v>73.33</v>
+        <v>73</v>
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="2" t="n">
+      <c r="A88" s="3" t="n">
         <v>45744</v>
       </c>
       <c r="B88" t="n">
-        <v>42.6</v>
+        <v>42</v>
       </c>
       <c r="C88" t="n">
-        <v>109.46</v>
+        <v>109</v>
       </c>
       <c r="D88" t="n">
-        <v>102.1</v>
+        <v>102</v>
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="2" t="n">
+      <c r="A89" s="3" t="n">
         <v>45745</v>
       </c>
       <c r="B89" t="n">
-        <v>40.1</v>
+        <v>40</v>
       </c>
       <c r="C89" t="n">
-        <v>98.54000000000001</v>
+        <v>98</v>
       </c>
       <c r="D89" t="n">
-        <v>109.46</v>
+        <v>109</v>
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="2" t="n">
+      <c r="A90" s="3" t="n">
         <v>45746</v>
       </c>
       <c r="B90" t="n">
-        <v>36.2</v>
+        <v>36</v>
       </c>
       <c r="C90" t="n">
-        <v>83.06</v>
+        <v>83</v>
       </c>
       <c r="D90" t="n">
-        <v>96.40000000000001</v>
+        <v>96</v>
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="2" t="n">
+      <c r="A91" s="3" t="n">
         <v>45747</v>
       </c>
       <c r="B91" t="n">
-        <v>41.8</v>
+        <v>41</v>
       </c>
       <c r="C91" t="n">
-        <v>69.7</v>
+        <v>69</v>
       </c>
       <c r="D91" t="n">
-        <v>74.06999999999999</v>
+        <v>74</v>
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="2" t="n">
+      <c r="A92" s="3" t="n">
         <v>45748</v>
       </c>
       <c r="B92" t="n">
-        <v>40.2</v>
+        <v>40</v>
       </c>
       <c r="C92" t="n">
-        <v>91.06999999999999</v>
+        <v>91</v>
       </c>
       <c r="D92" t="n">
-        <v>91.93000000000001</v>
+        <v>91</v>
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="2" t="n">
+      <c r="A93" s="3" t="n">
         <v>45749</v>
       </c>
       <c r="B93" t="n">
         <v>45</v>
       </c>
       <c r="C93" t="n">
-        <v>117.13</v>
+        <v>117</v>
       </c>
       <c r="D93" t="n">
-        <v>100.02</v>
+        <v>100</v>
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="2" t="n">
+      <c r="A94" s="3" t="n">
         <v>45750</v>
       </c>
       <c r="B94" t="n">
         <v>37</v>
       </c>
       <c r="C94" t="n">
-        <v>104.28</v>
+        <v>104</v>
       </c>
       <c r="D94" t="n">
-        <v>91.93000000000001</v>
+        <v>91</v>
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="2" t="n">
+      <c r="A95" s="3" t="n">
         <v>45751</v>
       </c>
       <c r="B95" t="n">
-        <v>39.3</v>
+        <v>39</v>
       </c>
       <c r="C95" t="n">
-        <v>75.09</v>
+        <v>75</v>
       </c>
       <c r="D95" t="n">
-        <v>102.26</v>
+        <v>102</v>
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="2" t="n">
+      <c r="A96" s="3" t="n">
         <v>45752</v>
       </c>
       <c r="B96" t="n">
-        <v>39.4</v>
+        <v>39</v>
       </c>
       <c r="C96" t="n">
-        <v>103.46</v>
+        <v>103</v>
       </c>
       <c r="D96" t="n">
-        <v>107.92</v>
+        <v>107</v>
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="2" t="n">
+      <c r="A97" s="3" t="n">
         <v>45753</v>
       </c>
       <c r="B97" t="n">
-        <v>34.5</v>
+        <v>34</v>
       </c>
       <c r="C97" t="n">
-        <v>107.71</v>
+        <v>107</v>
       </c>
       <c r="D97" t="n">
-        <v>91.84999999999999</v>
+        <v>91</v>
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="2" t="n">
+      <c r="A98" s="3" t="n">
         <v>45754</v>
       </c>
       <c r="B98" t="n">
-        <v>43.7</v>
+        <v>43</v>
       </c>
       <c r="C98" t="n">
-        <v>82.31999999999999</v>
+        <v>82</v>
       </c>
       <c r="D98" t="n">
-        <v>106.74</v>
+        <v>106</v>
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="2" t="n">
+      <c r="A99" s="3" t="n">
         <v>45755</v>
       </c>
       <c r="B99" t="n">
-        <v>43.9</v>
+        <v>43</v>
       </c>
       <c r="C99" t="n">
-        <v>103.07</v>
+        <v>103</v>
       </c>
       <c r="D99" t="n">
-        <v>106.86</v>
+        <v>106</v>
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="2" t="n">
+      <c r="A100" s="3" t="n">
         <v>45756</v>
       </c>
       <c r="B100" t="n">
-        <v>43.1</v>
+        <v>43</v>
       </c>
       <c r="C100" t="n">
-        <v>101.16</v>
+        <v>101</v>
       </c>
       <c r="D100" t="n">
-        <v>114.66</v>
+        <v>114</v>
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="2" t="n">
+      <c r="A101" s="3" t="n">
         <v>45757</v>
       </c>
       <c r="B101" t="n">
-        <v>42.3</v>
+        <v>42</v>
       </c>
       <c r="C101" t="n">
-        <v>77.14</v>
+        <v>77</v>
       </c>
       <c r="D101" t="n">
-        <v>99.48</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Set Excel number format to integer display (no decimals)
Values were already integers but Excel cell format may have
been showing decimal places.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/fake_data.xlsx
+++ b/fake_data.xlsx
@@ -51,11 +51,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -461,13 +462,13 @@
       <c r="A2" s="3" t="n">
         <v>45658</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" s="4" t="n">
         <v>71</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2" s="4" t="n">
         <v>92</v>
       </c>
     </row>
@@ -475,13 +476,13 @@
       <c r="A3" s="3" t="n">
         <v>45659</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" s="4" t="n">
         <v>91</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3" s="4" t="n">
         <v>105</v>
       </c>
     </row>
@@ -489,13 +490,13 @@
       <c r="A4" s="3" t="n">
         <v>45660</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" s="4" t="n">
         <v>93</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4" s="4" t="n">
         <v>115</v>
       </c>
     </row>
@@ -503,13 +504,13 @@
       <c r="A5" s="3" t="n">
         <v>45661</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5" s="4" t="n">
         <v>83</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5" s="4" t="n">
         <v>110</v>
       </c>
     </row>
@@ -517,13 +518,13 @@
       <c r="A6" s="3" t="n">
         <v>45662</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6" s="4" t="n">
         <v>96</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6" s="4" t="n">
         <v>74</v>
       </c>
     </row>
@@ -531,13 +532,13 @@
       <c r="A7" s="3" t="n">
         <v>45663</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7" s="4" t="n">
         <v>108</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7" s="4" t="n">
         <v>87</v>
       </c>
     </row>
@@ -545,13 +546,13 @@
       <c r="A8" s="3" t="n">
         <v>45664</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8" s="4" t="n">
         <v>137</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8" s="4" t="n">
         <v>127</v>
       </c>
     </row>
@@ -559,13 +560,13 @@
       <c r="A9" s="3" t="n">
         <v>45665</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9" s="4" t="n">
         <v>103</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9" s="4" t="n">
         <v>110</v>
       </c>
     </row>
@@ -573,13 +574,13 @@
       <c r="A10" s="3" t="n">
         <v>45666</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C10" s="4" t="n">
         <v>105</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D10" s="4" t="n">
         <v>111</v>
       </c>
     </row>
@@ -587,13 +588,13 @@
       <c r="A11" s="3" t="n">
         <v>45667</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="C11" t="n">
+      <c r="C11" s="4" t="n">
         <v>98</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D11" s="4" t="n">
         <v>165</v>
       </c>
     </row>
@@ -601,13 +602,13 @@
       <c r="A12" s="3" t="n">
         <v>45668</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C12" s="4" t="n">
         <v>61</v>
       </c>
-      <c r="D12" t="n">
+      <c r="D12" s="4" t="n">
         <v>90</v>
       </c>
     </row>
@@ -615,13 +616,13 @@
       <c r="A13" s="3" t="n">
         <v>45669</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="C13" t="n">
+      <c r="C13" s="4" t="n">
         <v>99</v>
       </c>
-      <c r="D13" t="n">
+      <c r="D13" s="4" t="n">
         <v>119</v>
       </c>
     </row>
@@ -629,13 +630,13 @@
       <c r="A14" s="3" t="n">
         <v>45670</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="C14" t="n">
+      <c r="C14" s="4" t="n">
         <v>101</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D14" s="4" t="n">
         <v>117</v>
       </c>
     </row>
@@ -643,13 +644,13 @@
       <c r="A15" s="3" t="n">
         <v>45671</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C15" s="4" t="n">
         <v>149</v>
       </c>
-      <c r="D15" t="n">
+      <c r="D15" s="4" t="n">
         <v>135</v>
       </c>
     </row>
@@ -657,13 +658,13 @@
       <c r="A16" s="3" t="n">
         <v>45672</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B16" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="C16" t="n">
+      <c r="C16" s="4" t="n">
         <v>96</v>
       </c>
-      <c r="D16" t="n">
+      <c r="D16" s="4" t="n">
         <v>92</v>
       </c>
     </row>
@@ -671,13 +672,13 @@
       <c r="A17" s="3" t="n">
         <v>45673</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B17" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="C17" t="n">
+      <c r="C17" s="4" t="n">
         <v>106</v>
       </c>
-      <c r="D17" t="n">
+      <c r="D17" s="4" t="n">
         <v>116</v>
       </c>
     </row>
@@ -685,13 +686,13 @@
       <c r="A18" s="3" t="n">
         <v>45674</v>
       </c>
-      <c r="B18" t="n">
+      <c r="B18" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="C18" t="n">
+      <c r="C18" s="4" t="n">
         <v>99</v>
       </c>
-      <c r="D18" t="n">
+      <c r="D18" s="4" t="n">
         <v>86</v>
       </c>
     </row>
@@ -699,13 +700,13 @@
       <c r="A19" s="3" t="n">
         <v>45675</v>
       </c>
-      <c r="B19" t="n">
+      <c r="B19" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="C19" t="n">
+      <c r="C19" s="4" t="n">
         <v>76</v>
       </c>
-      <c r="D19" t="n">
+      <c r="D19" s="4" t="n">
         <v>84</v>
       </c>
     </row>
@@ -713,13 +714,13 @@
       <c r="A20" s="3" t="n">
         <v>45676</v>
       </c>
-      <c r="B20" t="n">
+      <c r="B20" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="C20" t="n">
+      <c r="C20" s="4" t="n">
         <v>122</v>
       </c>
-      <c r="D20" t="n">
+      <c r="D20" s="4" t="n">
         <v>103</v>
       </c>
     </row>
@@ -727,13 +728,13 @@
       <c r="A21" s="3" t="n">
         <v>45677</v>
       </c>
-      <c r="B21" t="n">
+      <c r="B21" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="C21" t="n">
+      <c r="C21" s="4" t="n">
         <v>115</v>
       </c>
-      <c r="D21" t="n">
+      <c r="D21" s="4" t="n">
         <v>108</v>
       </c>
     </row>
@@ -741,13 +742,13 @@
       <c r="A22" s="3" t="n">
         <v>45678</v>
       </c>
-      <c r="B22" t="n">
+      <c r="B22" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="C22" t="n">
+      <c r="C22" s="4" t="n">
         <v>115</v>
       </c>
-      <c r="D22" t="n">
+      <c r="D22" s="4" t="n">
         <v>148</v>
       </c>
     </row>
@@ -755,13 +756,13 @@
       <c r="A23" s="3" t="n">
         <v>45679</v>
       </c>
-      <c r="B23" t="n">
+      <c r="B23" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="C23" t="n">
+      <c r="C23" s="4" t="n">
         <v>81</v>
       </c>
-      <c r="D23" t="n">
+      <c r="D23" s="4" t="n">
         <v>58</v>
       </c>
     </row>
@@ -769,13 +770,13 @@
       <c r="A24" s="3" t="n">
         <v>45680</v>
       </c>
-      <c r="B24" t="n">
+      <c r="B24" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="C24" t="n">
+      <c r="C24" s="4" t="n">
         <v>128</v>
       </c>
-      <c r="D24" t="n">
+      <c r="D24" s="4" t="n">
         <v>125</v>
       </c>
     </row>
@@ -783,13 +784,13 @@
       <c r="A25" s="3" t="n">
         <v>45681</v>
       </c>
-      <c r="B25" t="n">
+      <c r="B25" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="C25" t="n">
+      <c r="C25" s="4" t="n">
         <v>71</v>
       </c>
-      <c r="D25" t="n">
+      <c r="D25" s="4" t="n">
         <v>58</v>
       </c>
     </row>
@@ -797,13 +798,13 @@
       <c r="A26" s="3" t="n">
         <v>45682</v>
       </c>
-      <c r="B26" t="n">
+      <c r="B26" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="C26" t="n">
+      <c r="C26" s="4" t="n">
         <v>111</v>
       </c>
-      <c r="D26" t="n">
+      <c r="D26" s="4" t="n">
         <v>97</v>
       </c>
     </row>
@@ -811,13 +812,13 @@
       <c r="A27" s="3" t="n">
         <v>45683</v>
       </c>
-      <c r="B27" t="n">
+      <c r="B27" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="C27" t="n">
+      <c r="C27" s="4" t="n">
         <v>143</v>
       </c>
-      <c r="D27" t="n">
+      <c r="D27" s="4" t="n">
         <v>140</v>
       </c>
     </row>
@@ -825,13 +826,13 @@
       <c r="A28" s="3" t="n">
         <v>45684</v>
       </c>
-      <c r="B28" t="n">
+      <c r="B28" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="C28" t="n">
+      <c r="C28" s="4" t="n">
         <v>80</v>
       </c>
-      <c r="D28" t="n">
+      <c r="D28" s="4" t="n">
         <v>91</v>
       </c>
     </row>
@@ -839,13 +840,13 @@
       <c r="A29" s="3" t="n">
         <v>45685</v>
       </c>
-      <c r="B29" t="n">
+      <c r="B29" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="C29" t="n">
+      <c r="C29" s="4" t="n">
         <v>88</v>
       </c>
-      <c r="D29" t="n">
+      <c r="D29" s="4" t="n">
         <v>75</v>
       </c>
     </row>
@@ -853,13 +854,13 @@
       <c r="A30" s="3" t="n">
         <v>45686</v>
       </c>
-      <c r="B30" t="n">
+      <c r="B30" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="C30" t="n">
+      <c r="C30" s="4" t="n">
         <v>101</v>
       </c>
-      <c r="D30" t="n">
+      <c r="D30" s="4" t="n">
         <v>88</v>
       </c>
     </row>
@@ -867,13 +868,13 @@
       <c r="A31" s="3" t="n">
         <v>45687</v>
       </c>
-      <c r="B31" t="n">
+      <c r="B31" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="C31" t="n">
+      <c r="C31" s="4" t="n">
         <v>89</v>
       </c>
-      <c r="D31" t="n">
+      <c r="D31" s="4" t="n">
         <v>106</v>
       </c>
     </row>
@@ -881,13 +882,13 @@
       <c r="A32" s="3" t="n">
         <v>45688</v>
       </c>
-      <c r="B32" t="n">
+      <c r="B32" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="C32" t="n">
+      <c r="C32" s="4" t="n">
         <v>68</v>
       </c>
-      <c r="D32" t="n">
+      <c r="D32" s="4" t="n">
         <v>71</v>
       </c>
     </row>
@@ -895,13 +896,13 @@
       <c r="A33" s="3" t="n">
         <v>45689</v>
       </c>
-      <c r="B33" t="n">
+      <c r="B33" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="C33" t="n">
+      <c r="C33" s="4" t="n">
         <v>101</v>
       </c>
-      <c r="D33" t="n">
+      <c r="D33" s="4" t="n">
         <v>104</v>
       </c>
     </row>
@@ -909,13 +910,13 @@
       <c r="A34" s="3" t="n">
         <v>45690</v>
       </c>
-      <c r="B34" t="n">
+      <c r="B34" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="C34" t="n">
+      <c r="C34" s="4" t="n">
         <v>78</v>
       </c>
-      <c r="D34" t="n">
+      <c r="D34" s="4" t="n">
         <v>90</v>
       </c>
     </row>
@@ -923,13 +924,13 @@
       <c r="A35" s="3" t="n">
         <v>45691</v>
       </c>
-      <c r="B35" t="n">
+      <c r="B35" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="C35" t="n">
+      <c r="C35" s="4" t="n">
         <v>109</v>
       </c>
-      <c r="D35" t="n">
+      <c r="D35" s="4" t="n">
         <v>93</v>
       </c>
     </row>
@@ -937,13 +938,13 @@
       <c r="A36" s="3" t="n">
         <v>45692</v>
       </c>
-      <c r="B36" t="n">
+      <c r="B36" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="C36" t="n">
+      <c r="C36" s="4" t="n">
         <v>81</v>
       </c>
-      <c r="D36" t="n">
+      <c r="D36" s="4" t="n">
         <v>127</v>
       </c>
     </row>
@@ -951,13 +952,13 @@
       <c r="A37" s="3" t="n">
         <v>45693</v>
       </c>
-      <c r="B37" t="n">
+      <c r="B37" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="C37" t="n">
+      <c r="C37" s="4" t="n">
         <v>131</v>
       </c>
-      <c r="D37" t="n">
+      <c r="D37" s="4" t="n">
         <v>126</v>
       </c>
     </row>
@@ -965,13 +966,13 @@
       <c r="A38" s="3" t="n">
         <v>45694</v>
       </c>
-      <c r="B38" t="n">
+      <c r="B38" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="C38" t="n">
+      <c r="C38" s="4" t="n">
         <v>84</v>
       </c>
-      <c r="D38" t="n">
+      <c r="D38" s="4" t="n">
         <v>57</v>
       </c>
     </row>
@@ -979,13 +980,13 @@
       <c r="A39" s="3" t="n">
         <v>45695</v>
       </c>
-      <c r="B39" t="n">
+      <c r="B39" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="C39" t="n">
+      <c r="C39" s="4" t="n">
         <v>93</v>
       </c>
-      <c r="D39" t="n">
+      <c r="D39" s="4" t="n">
         <v>100</v>
       </c>
     </row>
@@ -993,13 +994,13 @@
       <c r="A40" s="3" t="n">
         <v>45696</v>
       </c>
-      <c r="B40" t="n">
+      <c r="B40" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="C40" t="n">
+      <c r="C40" s="4" t="n">
         <v>116</v>
       </c>
-      <c r="D40" t="n">
+      <c r="D40" s="4" t="n">
         <v>96</v>
       </c>
     </row>
@@ -1007,13 +1008,13 @@
       <c r="A41" s="3" t="n">
         <v>45697</v>
       </c>
-      <c r="B41" t="n">
+      <c r="B41" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="C41" t="n">
+      <c r="C41" s="4" t="n">
         <v>75</v>
       </c>
-      <c r="D41" t="n">
+      <c r="D41" s="4" t="n">
         <v>102</v>
       </c>
     </row>
@@ -1021,13 +1022,13 @@
       <c r="A42" s="3" t="n">
         <v>45698</v>
       </c>
-      <c r="B42" t="n">
+      <c r="B42" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="C42" t="n">
+      <c r="C42" s="4" t="n">
         <v>104</v>
       </c>
-      <c r="D42" t="n">
+      <c r="D42" s="4" t="n">
         <v>88</v>
       </c>
     </row>
@@ -1035,13 +1036,13 @@
       <c r="A43" s="3" t="n">
         <v>45699</v>
       </c>
-      <c r="B43" t="n">
+      <c r="B43" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="C43" t="n">
+      <c r="C43" s="4" t="n">
         <v>126</v>
       </c>
-      <c r="D43" t="n">
+      <c r="D43" s="4" t="n">
         <v>111</v>
       </c>
     </row>
@@ -1049,13 +1050,13 @@
       <c r="A44" s="3" t="n">
         <v>45700</v>
       </c>
-      <c r="B44" t="n">
+      <c r="B44" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="C44" t="n">
+      <c r="C44" s="4" t="n">
         <v>67</v>
       </c>
-      <c r="D44" t="n">
+      <c r="D44" s="4" t="n">
         <v>92</v>
       </c>
     </row>
@@ -1063,13 +1064,13 @@
       <c r="A45" s="3" t="n">
         <v>45701</v>
       </c>
-      <c r="B45" t="n">
+      <c r="B45" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="C45" t="n">
+      <c r="C45" s="4" t="n">
         <v>103</v>
       </c>
-      <c r="D45" t="n">
+      <c r="D45" s="4" t="n">
         <v>116</v>
       </c>
     </row>
@@ -1077,13 +1078,13 @@
       <c r="A46" s="3" t="n">
         <v>45702</v>
       </c>
-      <c r="B46" t="n">
+      <c r="B46" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="C46" t="n">
+      <c r="C46" s="4" t="n">
         <v>105</v>
       </c>
-      <c r="D46" t="n">
+      <c r="D46" s="4" t="n">
         <v>81</v>
       </c>
     </row>
@@ -1091,13 +1092,13 @@
       <c r="A47" s="3" t="n">
         <v>45703</v>
       </c>
-      <c r="B47" t="n">
+      <c r="B47" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="C47" t="n">
+      <c r="C47" s="4" t="n">
         <v>115</v>
       </c>
-      <c r="D47" t="n">
+      <c r="D47" s="4" t="n">
         <v>102</v>
       </c>
     </row>
@@ -1105,13 +1106,13 @@
       <c r="A48" s="3" t="n">
         <v>45704</v>
       </c>
-      <c r="B48" t="n">
+      <c r="B48" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="C48" t="n">
+      <c r="C48" s="4" t="n">
         <v>75</v>
       </c>
-      <c r="D48" t="n">
+      <c r="D48" s="4" t="n">
         <v>79</v>
       </c>
     </row>
@@ -1119,13 +1120,13 @@
       <c r="A49" s="3" t="n">
         <v>45705</v>
       </c>
-      <c r="B49" t="n">
+      <c r="B49" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="C49" t="n">
+      <c r="C49" s="4" t="n">
         <v>73</v>
       </c>
-      <c r="D49" t="n">
+      <c r="D49" s="4" t="n">
         <v>75</v>
       </c>
     </row>
@@ -1133,13 +1134,13 @@
       <c r="A50" s="3" t="n">
         <v>45706</v>
       </c>
-      <c r="B50" t="n">
+      <c r="B50" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="C50" t="n">
+      <c r="C50" s="4" t="n">
         <v>110</v>
       </c>
-      <c r="D50" t="n">
+      <c r="D50" s="4" t="n">
         <v>135</v>
       </c>
     </row>
@@ -1147,13 +1148,13 @@
       <c r="A51" s="3" t="n">
         <v>45707</v>
       </c>
-      <c r="B51" t="n">
+      <c r="B51" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="C51" t="n">
+      <c r="C51" s="4" t="n">
         <v>105</v>
       </c>
-      <c r="D51" t="n">
+      <c r="D51" s="4" t="n">
         <v>109</v>
       </c>
     </row>
@@ -1161,13 +1162,13 @@
       <c r="A52" s="3" t="n">
         <v>45708</v>
       </c>
-      <c r="B52" t="n">
+      <c r="B52" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="C52" t="n">
+      <c r="C52" s="4" t="n">
         <v>105</v>
       </c>
-      <c r="D52" t="n">
+      <c r="D52" s="4" t="n">
         <v>80</v>
       </c>
     </row>
@@ -1175,13 +1176,13 @@
       <c r="A53" s="3" t="n">
         <v>45709</v>
       </c>
-      <c r="B53" t="n">
+      <c r="B53" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="C53" t="n">
+      <c r="C53" s="4" t="n">
         <v>106</v>
       </c>
-      <c r="D53" t="n">
+      <c r="D53" s="4" t="n">
         <v>119</v>
       </c>
     </row>
@@ -1189,13 +1190,13 @@
       <c r="A54" s="3" t="n">
         <v>45710</v>
       </c>
-      <c r="B54" t="n">
+      <c r="B54" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="C54" t="n">
+      <c r="C54" s="4" t="n">
         <v>86</v>
       </c>
-      <c r="D54" t="n">
+      <c r="D54" s="4" t="n">
         <v>129</v>
       </c>
     </row>
@@ -1203,13 +1204,13 @@
       <c r="A55" s="3" t="n">
         <v>45711</v>
       </c>
-      <c r="B55" t="n">
+      <c r="B55" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="C55" t="n">
+      <c r="C55" s="4" t="n">
         <v>104</v>
       </c>
-      <c r="D55" t="n">
+      <c r="D55" s="4" t="n">
         <v>120</v>
       </c>
     </row>
@@ -1217,13 +1218,13 @@
       <c r="A56" s="3" t="n">
         <v>45712</v>
       </c>
-      <c r="B56" t="n">
+      <c r="B56" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="C56" t="n">
+      <c r="C56" s="4" t="n">
         <v>105</v>
       </c>
-      <c r="D56" t="n">
+      <c r="D56" s="4" t="n">
         <v>76</v>
       </c>
     </row>
@@ -1231,13 +1232,13 @@
       <c r="A57" s="3" t="n">
         <v>45713</v>
       </c>
-      <c r="B57" t="n">
+      <c r="B57" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="C57" t="n">
+      <c r="C57" s="4" t="n">
         <v>85</v>
       </c>
-      <c r="D57" t="n">
+      <c r="D57" s="4" t="n">
         <v>84</v>
       </c>
     </row>
@@ -1245,13 +1246,13 @@
       <c r="A58" s="3" t="n">
         <v>45714</v>
       </c>
-      <c r="B58" t="n">
+      <c r="B58" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="C58" t="n">
+      <c r="C58" s="4" t="n">
         <v>137</v>
       </c>
-      <c r="D58" t="n">
+      <c r="D58" s="4" t="n">
         <v>140</v>
       </c>
     </row>
@@ -1259,13 +1260,13 @@
       <c r="A59" s="3" t="n">
         <v>45715</v>
       </c>
-      <c r="B59" t="n">
+      <c r="B59" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="C59" t="n">
+      <c r="C59" s="4" t="n">
         <v>109</v>
       </c>
-      <c r="D59" t="n">
+      <c r="D59" s="4" t="n">
         <v>92</v>
       </c>
     </row>
@@ -1273,13 +1274,13 @@
       <c r="A60" s="3" t="n">
         <v>45716</v>
       </c>
-      <c r="B60" t="n">
+      <c r="B60" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="C60" t="n">
+      <c r="C60" s="4" t="n">
         <v>76</v>
       </c>
-      <c r="D60" t="n">
+      <c r="D60" s="4" t="n">
         <v>95</v>
       </c>
     </row>
@@ -1287,13 +1288,13 @@
       <c r="A61" s="3" t="n">
         <v>45717</v>
       </c>
-      <c r="B61" t="n">
+      <c r="B61" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="C61" t="n">
+      <c r="C61" s="4" t="n">
         <v>113</v>
       </c>
-      <c r="D61" t="n">
+      <c r="D61" s="4" t="n">
         <v>119</v>
       </c>
     </row>
@@ -1301,13 +1302,13 @@
       <c r="A62" s="3" t="n">
         <v>45718</v>
       </c>
-      <c r="B62" t="n">
+      <c r="B62" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="C62" t="n">
+      <c r="C62" s="4" t="n">
         <v>80</v>
       </c>
-      <c r="D62" t="n">
+      <c r="D62" s="4" t="n">
         <v>74</v>
       </c>
     </row>
@@ -1315,13 +1316,13 @@
       <c r="A63" s="3" t="n">
         <v>45719</v>
       </c>
-      <c r="B63" t="n">
+      <c r="B63" s="4" t="n">
         <v>26</v>
       </c>
-      <c r="C63" t="n">
+      <c r="C63" s="4" t="n">
         <v>115</v>
       </c>
-      <c r="D63" t="n">
+      <c r="D63" s="4" t="n">
         <v>106</v>
       </c>
     </row>
@@ -1329,13 +1330,13 @@
       <c r="A64" s="3" t="n">
         <v>45720</v>
       </c>
-      <c r="B64" t="n">
+      <c r="B64" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="C64" t="n">
+      <c r="C64" s="4" t="n">
         <v>123</v>
       </c>
-      <c r="D64" t="n">
+      <c r="D64" s="4" t="n">
         <v>55</v>
       </c>
     </row>
@@ -1343,13 +1344,13 @@
       <c r="A65" s="3" t="n">
         <v>45721</v>
       </c>
-      <c r="B65" t="n">
+      <c r="B65" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="C65" t="n">
+      <c r="C65" s="4" t="n">
         <v>83</v>
       </c>
-      <c r="D65" t="n">
+      <c r="D65" s="4" t="n">
         <v>74</v>
       </c>
     </row>
@@ -1357,13 +1358,13 @@
       <c r="A66" s="3" t="n">
         <v>45722</v>
       </c>
-      <c r="B66" t="n">
+      <c r="B66" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="C66" t="n">
+      <c r="C66" s="4" t="n">
         <v>119</v>
       </c>
-      <c r="D66" t="n">
+      <c r="D66" s="4" t="n">
         <v>105</v>
       </c>
     </row>
@@ -1371,13 +1372,13 @@
       <c r="A67" s="3" t="n">
         <v>45723</v>
       </c>
-      <c r="B67" t="n">
+      <c r="B67" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="C67" t="n">
+      <c r="C67" s="4" t="n">
         <v>108</v>
       </c>
-      <c r="D67" t="n">
+      <c r="D67" s="4" t="n">
         <v>82</v>
       </c>
     </row>
@@ -1385,13 +1386,13 @@
       <c r="A68" s="3" t="n">
         <v>45724</v>
       </c>
-      <c r="B68" t="n">
+      <c r="B68" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="C68" t="n">
+      <c r="C68" s="4" t="n">
         <v>116</v>
       </c>
-      <c r="D68" t="n">
+      <c r="D68" s="4" t="n">
         <v>136</v>
       </c>
     </row>
@@ -1399,13 +1400,13 @@
       <c r="A69" s="3" t="n">
         <v>45725</v>
       </c>
-      <c r="B69" t="n">
+      <c r="B69" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="C69" t="n">
+      <c r="C69" s="4" t="n">
         <v>137</v>
       </c>
-      <c r="D69" t="n">
+      <c r="D69" s="4" t="n">
         <v>94</v>
       </c>
     </row>
@@ -1413,13 +1414,13 @@
       <c r="A70" s="3" t="n">
         <v>45726</v>
       </c>
-      <c r="B70" t="n">
+      <c r="B70" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="C70" t="n">
+      <c r="C70" s="4" t="n">
         <v>95</v>
       </c>
-      <c r="D70" t="n">
+      <c r="D70" s="4" t="n">
         <v>89</v>
       </c>
     </row>
@@ -1427,13 +1428,13 @@
       <c r="A71" s="3" t="n">
         <v>45727</v>
       </c>
-      <c r="B71" t="n">
+      <c r="B71" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="C71" t="n">
+      <c r="C71" s="4" t="n">
         <v>84</v>
       </c>
-      <c r="D71" t="n">
+      <c r="D71" s="4" t="n">
         <v>94</v>
       </c>
     </row>
@@ -1441,13 +1442,13 @@
       <c r="A72" s="3" t="n">
         <v>45728</v>
       </c>
-      <c r="B72" t="n">
+      <c r="B72" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="C72" t="n">
+      <c r="C72" s="4" t="n">
         <v>82</v>
       </c>
-      <c r="D72" t="n">
+      <c r="D72" s="4" t="n">
         <v>116</v>
       </c>
     </row>
@@ -1455,13 +1456,13 @@
       <c r="A73" s="3" t="n">
         <v>45729</v>
       </c>
-      <c r="B73" t="n">
+      <c r="B73" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="C73" t="n">
+      <c r="C73" s="4" t="n">
         <v>83</v>
       </c>
-      <c r="D73" t="n">
+      <c r="D73" s="4" t="n">
         <v>66</v>
       </c>
     </row>
@@ -1469,13 +1470,13 @@
       <c r="A74" s="3" t="n">
         <v>45730</v>
       </c>
-      <c r="B74" t="n">
+      <c r="B74" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="C74" t="n">
+      <c r="C74" s="4" t="n">
         <v>98</v>
       </c>
-      <c r="D74" t="n">
+      <c r="D74" s="4" t="n">
         <v>119</v>
       </c>
     </row>
@@ -1483,13 +1484,13 @@
       <c r="A75" s="3" t="n">
         <v>45731</v>
       </c>
-      <c r="B75" t="n">
+      <c r="B75" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="C75" t="n">
+      <c r="C75" s="4" t="n">
         <v>106</v>
       </c>
-      <c r="D75" t="n">
+      <c r="D75" s="4" t="n">
         <v>103</v>
       </c>
     </row>
@@ -1497,13 +1498,13 @@
       <c r="A76" s="3" t="n">
         <v>45732</v>
       </c>
-      <c r="B76" t="n">
+      <c r="B76" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="C76" t="n">
+      <c r="C76" s="4" t="n">
         <v>105</v>
       </c>
-      <c r="D76" t="n">
+      <c r="D76" s="4" t="n">
         <v>85</v>
       </c>
     </row>
@@ -1511,13 +1512,13 @@
       <c r="A77" s="3" t="n">
         <v>45733</v>
       </c>
-      <c r="B77" t="n">
+      <c r="B77" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="C77" t="n">
+      <c r="C77" s="4" t="n">
         <v>116</v>
       </c>
-      <c r="D77" t="n">
+      <c r="D77" s="4" t="n">
         <v>116</v>
       </c>
     </row>
@@ -1525,13 +1526,13 @@
       <c r="A78" s="3" t="n">
         <v>45734</v>
       </c>
-      <c r="B78" t="n">
+      <c r="B78" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="C78" t="n">
+      <c r="C78" s="4" t="n">
         <v>100</v>
       </c>
-      <c r="D78" t="n">
+      <c r="D78" s="4" t="n">
         <v>103</v>
       </c>
     </row>
@@ -1539,13 +1540,13 @@
       <c r="A79" s="3" t="n">
         <v>45735</v>
       </c>
-      <c r="B79" t="n">
+      <c r="B79" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="C79" t="n">
+      <c r="C79" s="4" t="n">
         <v>129</v>
       </c>
-      <c r="D79" t="n">
+      <c r="D79" s="4" t="n">
         <v>104</v>
       </c>
     </row>
@@ -1553,13 +1554,13 @@
       <c r="A80" s="3" t="n">
         <v>45736</v>
       </c>
-      <c r="B80" t="n">
+      <c r="B80" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="C80" t="n">
+      <c r="C80" s="4" t="n">
         <v>94</v>
       </c>
-      <c r="D80" t="n">
+      <c r="D80" s="4" t="n">
         <v>98</v>
       </c>
     </row>
@@ -1567,13 +1568,13 @@
       <c r="A81" s="3" t="n">
         <v>45737</v>
       </c>
-      <c r="B81" t="n">
+      <c r="B81" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="C81" t="n">
+      <c r="C81" s="4" t="n">
         <v>154</v>
       </c>
-      <c r="D81" t="n">
+      <c r="D81" s="4" t="n">
         <v>120</v>
       </c>
     </row>
@@ -1581,13 +1582,13 @@
       <c r="A82" s="3" t="n">
         <v>45738</v>
       </c>
-      <c r="B82" t="n">
+      <c r="B82" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="C82" t="n">
+      <c r="C82" s="4" t="n">
         <v>112</v>
       </c>
-      <c r="D82" t="n">
+      <c r="D82" s="4" t="n">
         <v>108</v>
       </c>
     </row>
@@ -1595,13 +1596,13 @@
       <c r="A83" s="3" t="n">
         <v>45739</v>
       </c>
-      <c r="B83" t="n">
+      <c r="B83" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="C83" t="n">
+      <c r="C83" s="4" t="n">
         <v>82</v>
       </c>
-      <c r="D83" t="n">
+      <c r="D83" s="4" t="n">
         <v>102</v>
       </c>
     </row>
@@ -1609,13 +1610,13 @@
       <c r="A84" s="3" t="n">
         <v>45740</v>
       </c>
-      <c r="B84" t="n">
+      <c r="B84" s="4" t="n">
         <v>43</v>
       </c>
-      <c r="C84" t="n">
+      <c r="C84" s="4" t="n">
         <v>78</v>
       </c>
-      <c r="D84" t="n">
+      <c r="D84" s="4" t="n">
         <v>116</v>
       </c>
     </row>
@@ -1623,13 +1624,13 @@
       <c r="A85" s="3" t="n">
         <v>45741</v>
       </c>
-      <c r="B85" t="n">
+      <c r="B85" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="C85" t="n">
+      <c r="C85" s="4" t="n">
         <v>109</v>
       </c>
-      <c r="D85" t="n">
+      <c r="D85" s="4" t="n">
         <v>83</v>
       </c>
     </row>
@@ -1637,13 +1638,13 @@
       <c r="A86" s="3" t="n">
         <v>45742</v>
       </c>
-      <c r="B86" t="n">
+      <c r="B86" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="C86" t="n">
+      <c r="C86" s="4" t="n">
         <v>95</v>
       </c>
-      <c r="D86" t="n">
+      <c r="D86" s="4" t="n">
         <v>134</v>
       </c>
     </row>
@@ -1651,13 +1652,13 @@
       <c r="A87" s="3" t="n">
         <v>45743</v>
       </c>
-      <c r="B87" t="n">
+      <c r="B87" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="C87" t="n">
+      <c r="C87" s="4" t="n">
         <v>114</v>
       </c>
-      <c r="D87" t="n">
+      <c r="D87" s="4" t="n">
         <v>73</v>
       </c>
     </row>
@@ -1665,13 +1666,13 @@
       <c r="A88" s="3" t="n">
         <v>45744</v>
       </c>
-      <c r="B88" t="n">
+      <c r="B88" s="4" t="n">
         <v>42</v>
       </c>
-      <c r="C88" t="n">
+      <c r="C88" s="4" t="n">
         <v>109</v>
       </c>
-      <c r="D88" t="n">
+      <c r="D88" s="4" t="n">
         <v>102</v>
       </c>
     </row>
@@ -1679,13 +1680,13 @@
       <c r="A89" s="3" t="n">
         <v>45745</v>
       </c>
-      <c r="B89" t="n">
+      <c r="B89" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="C89" t="n">
+      <c r="C89" s="4" t="n">
         <v>98</v>
       </c>
-      <c r="D89" t="n">
+      <c r="D89" s="4" t="n">
         <v>109</v>
       </c>
     </row>
@@ -1693,13 +1694,13 @@
       <c r="A90" s="3" t="n">
         <v>45746</v>
       </c>
-      <c r="B90" t="n">
+      <c r="B90" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="C90" t="n">
+      <c r="C90" s="4" t="n">
         <v>83</v>
       </c>
-      <c r="D90" t="n">
+      <c r="D90" s="4" t="n">
         <v>96</v>
       </c>
     </row>
@@ -1707,13 +1708,13 @@
       <c r="A91" s="3" t="n">
         <v>45747</v>
       </c>
-      <c r="B91" t="n">
+      <c r="B91" s="4" t="n">
         <v>41</v>
       </c>
-      <c r="C91" t="n">
+      <c r="C91" s="4" t="n">
         <v>69</v>
       </c>
-      <c r="D91" t="n">
+      <c r="D91" s="4" t="n">
         <v>74</v>
       </c>
     </row>
@@ -1721,13 +1722,13 @@
       <c r="A92" s="3" t="n">
         <v>45748</v>
       </c>
-      <c r="B92" t="n">
+      <c r="B92" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="C92" t="n">
+      <c r="C92" s="4" t="n">
         <v>91</v>
       </c>
-      <c r="D92" t="n">
+      <c r="D92" s="4" t="n">
         <v>91</v>
       </c>
     </row>
@@ -1735,13 +1736,13 @@
       <c r="A93" s="3" t="n">
         <v>45749</v>
       </c>
-      <c r="B93" t="n">
+      <c r="B93" s="4" t="n">
         <v>45</v>
       </c>
-      <c r="C93" t="n">
+      <c r="C93" s="4" t="n">
         <v>117</v>
       </c>
-      <c r="D93" t="n">
+      <c r="D93" s="4" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1749,13 +1750,13 @@
       <c r="A94" s="3" t="n">
         <v>45750</v>
       </c>
-      <c r="B94" t="n">
+      <c r="B94" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="C94" t="n">
+      <c r="C94" s="4" t="n">
         <v>104</v>
       </c>
-      <c r="D94" t="n">
+      <c r="D94" s="4" t="n">
         <v>91</v>
       </c>
     </row>
@@ -1763,13 +1764,13 @@
       <c r="A95" s="3" t="n">
         <v>45751</v>
       </c>
-      <c r="B95" t="n">
+      <c r="B95" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="C95" t="n">
+      <c r="C95" s="4" t="n">
         <v>75</v>
       </c>
-      <c r="D95" t="n">
+      <c r="D95" s="4" t="n">
         <v>102</v>
       </c>
     </row>
@@ -1777,13 +1778,13 @@
       <c r="A96" s="3" t="n">
         <v>45752</v>
       </c>
-      <c r="B96" t="n">
+      <c r="B96" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="C96" t="n">
+      <c r="C96" s="4" t="n">
         <v>103</v>
       </c>
-      <c r="D96" t="n">
+      <c r="D96" s="4" t="n">
         <v>107</v>
       </c>
     </row>
@@ -1791,13 +1792,13 @@
       <c r="A97" s="3" t="n">
         <v>45753</v>
       </c>
-      <c r="B97" t="n">
+      <c r="B97" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="C97" t="n">
+      <c r="C97" s="4" t="n">
         <v>107</v>
       </c>
-      <c r="D97" t="n">
+      <c r="D97" s="4" t="n">
         <v>91</v>
       </c>
     </row>
@@ -1805,13 +1806,13 @@
       <c r="A98" s="3" t="n">
         <v>45754</v>
       </c>
-      <c r="B98" t="n">
+      <c r="B98" s="4" t="n">
         <v>43</v>
       </c>
-      <c r="C98" t="n">
+      <c r="C98" s="4" t="n">
         <v>82</v>
       </c>
-      <c r="D98" t="n">
+      <c r="D98" s="4" t="n">
         <v>106</v>
       </c>
     </row>
@@ -1819,13 +1820,13 @@
       <c r="A99" s="3" t="n">
         <v>45755</v>
       </c>
-      <c r="B99" t="n">
+      <c r="B99" s="4" t="n">
         <v>43</v>
       </c>
-      <c r="C99" t="n">
+      <c r="C99" s="4" t="n">
         <v>103</v>
       </c>
-      <c r="D99" t="n">
+      <c r="D99" s="4" t="n">
         <v>106</v>
       </c>
     </row>
@@ -1833,13 +1834,13 @@
       <c r="A100" s="3" t="n">
         <v>45756</v>
       </c>
-      <c r="B100" t="n">
+      <c r="B100" s="4" t="n">
         <v>43</v>
       </c>
-      <c r="C100" t="n">
+      <c r="C100" s="4" t="n">
         <v>101</v>
       </c>
-      <c r="D100" t="n">
+      <c r="D100" s="4" t="n">
         <v>114</v>
       </c>
     </row>
@@ -1847,13 +1848,13 @@
       <c r="A101" s="3" t="n">
         <v>45757</v>
       </c>
-      <c r="B101" t="n">
+      <c r="B101" s="4" t="n">
         <v>42</v>
       </c>
-      <c r="C101" t="n">
+      <c r="C101" s="4" t="n">
         <v>77</v>
       </c>
-      <c r="D101" t="n">
+      <c r="D101" s="4" t="n">
         <v>99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add tenths of degrees to temperature column in fake_data.xlsx
Temperature now has one decimal place (e.g. 13.6 F). Variable_1
and Variable_2 remain integers. HTML preview table updated to match.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/fake_data.xlsx
+++ b/fake_data.xlsx
@@ -16,8 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -51,12 +52,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -462,8 +464,8 @@
       <c r="A2" s="3" t="n">
         <v>45658</v>
       </c>
-      <c r="B2" s="4" t="n">
-        <v>13</v>
+      <c r="B2" s="5" t="n">
+        <v>13.6</v>
       </c>
       <c r="C2" s="4" t="n">
         <v>71</v>
@@ -476,7 +478,7 @@
       <c r="A3" s="3" t="n">
         <v>45659</v>
       </c>
-      <c r="B3" s="4" t="n">
+      <c r="B3" s="5" t="n">
         <v>10</v>
       </c>
       <c r="C3" s="4" t="n">
@@ -490,8 +492,8 @@
       <c r="A4" s="3" t="n">
         <v>45660</v>
       </c>
-      <c r="B4" s="4" t="n">
-        <v>14</v>
+      <c r="B4" s="5" t="n">
+        <v>14.2</v>
       </c>
       <c r="C4" s="4" t="n">
         <v>93</v>
@@ -504,8 +506,8 @@
       <c r="A5" s="3" t="n">
         <v>45661</v>
       </c>
-      <c r="B5" s="4" t="n">
-        <v>18</v>
+      <c r="B5" s="5" t="n">
+        <v>18.2</v>
       </c>
       <c r="C5" s="4" t="n">
         <v>83</v>
@@ -518,8 +520,8 @@
       <c r="A6" s="3" t="n">
         <v>45662</v>
       </c>
-      <c r="B6" s="4" t="n">
-        <v>9</v>
+      <c r="B6" s="5" t="n">
+        <v>9.699999999999999</v>
       </c>
       <c r="C6" s="4" t="n">
         <v>96</v>
@@ -532,8 +534,8 @@
       <c r="A7" s="3" t="n">
         <v>45663</v>
       </c>
-      <c r="B7" s="4" t="n">
-        <v>9</v>
+      <c r="B7" s="5" t="n">
+        <v>9.6</v>
       </c>
       <c r="C7" s="4" t="n">
         <v>108</v>
@@ -546,8 +548,8 @@
       <c r="A8" s="3" t="n">
         <v>45664</v>
       </c>
-      <c r="B8" s="4" t="n">
-        <v>19</v>
+      <c r="B8" s="5" t="n">
+        <v>19.8</v>
       </c>
       <c r="C8" s="4" t="n">
         <v>137</v>
@@ -560,8 +562,8 @@
       <c r="A9" s="3" t="n">
         <v>45665</v>
       </c>
-      <c r="B9" s="4" t="n">
-        <v>15</v>
+      <c r="B9" s="5" t="n">
+        <v>15.1</v>
       </c>
       <c r="C9" s="4" t="n">
         <v>103</v>
@@ -574,8 +576,8 @@
       <c r="A10" s="3" t="n">
         <v>45666</v>
       </c>
-      <c r="B10" s="4" t="n">
-        <v>9</v>
+      <c r="B10" s="5" t="n">
+        <v>9.4</v>
       </c>
       <c r="C10" s="4" t="n">
         <v>105</v>
@@ -588,7 +590,7 @@
       <c r="A11" s="3" t="n">
         <v>45667</v>
       </c>
-      <c r="B11" s="4" t="n">
+      <c r="B11" s="5" t="n">
         <v>14</v>
       </c>
       <c r="C11" s="4" t="n">
@@ -602,8 +604,8 @@
       <c r="A12" s="3" t="n">
         <v>45668</v>
       </c>
-      <c r="B12" s="4" t="n">
-        <v>9</v>
+      <c r="B12" s="5" t="n">
+        <v>9.199999999999999</v>
       </c>
       <c r="C12" s="4" t="n">
         <v>61</v>
@@ -616,8 +618,8 @@
       <c r="A13" s="3" t="n">
         <v>45669</v>
       </c>
-      <c r="B13" s="4" t="n">
-        <v>9</v>
+      <c r="B13" s="5" t="n">
+        <v>9.5</v>
       </c>
       <c r="C13" s="4" t="n">
         <v>99</v>
@@ -630,7 +632,7 @@
       <c r="A14" s="3" t="n">
         <v>45670</v>
       </c>
-      <c r="B14" s="4" t="n">
+      <c r="B14" s="5" t="n">
         <v>13</v>
       </c>
       <c r="C14" s="4" t="n">
@@ -644,8 +646,8 @@
       <c r="A15" s="3" t="n">
         <v>45671</v>
       </c>
-      <c r="B15" s="4" t="n">
-        <v>2</v>
+      <c r="B15" s="5" t="n">
+        <v>2.2</v>
       </c>
       <c r="C15" s="4" t="n">
         <v>149</v>
@@ -658,8 +660,8 @@
       <c r="A16" s="3" t="n">
         <v>45672</v>
       </c>
-      <c r="B16" s="4" t="n">
-        <v>3</v>
+      <c r="B16" s="5" t="n">
+        <v>3.6</v>
       </c>
       <c r="C16" s="4" t="n">
         <v>96</v>
@@ -672,8 +674,8 @@
       <c r="A17" s="3" t="n">
         <v>45673</v>
       </c>
-      <c r="B17" s="4" t="n">
-        <v>9</v>
+      <c r="B17" s="5" t="n">
+        <v>9.5</v>
       </c>
       <c r="C17" s="4" t="n">
         <v>106</v>
@@ -686,8 +688,8 @@
       <c r="A18" s="3" t="n">
         <v>45674</v>
       </c>
-      <c r="B18" s="4" t="n">
-        <v>7</v>
+      <c r="B18" s="5" t="n">
+        <v>7.2</v>
       </c>
       <c r="C18" s="4" t="n">
         <v>99</v>
@@ -700,8 +702,8 @@
       <c r="A19" s="3" t="n">
         <v>45675</v>
       </c>
-      <c r="B19" s="4" t="n">
-        <v>14</v>
+      <c r="B19" s="5" t="n">
+        <v>14.5</v>
       </c>
       <c r="C19" s="4" t="n">
         <v>76</v>
@@ -714,8 +716,8 @@
       <c r="A20" s="3" t="n">
         <v>45676</v>
       </c>
-      <c r="B20" s="4" t="n">
-        <v>8</v>
+      <c r="B20" s="5" t="n">
+        <v>8.699999999999999</v>
       </c>
       <c r="C20" s="4" t="n">
         <v>122</v>
@@ -728,7 +730,7 @@
       <c r="A21" s="3" t="n">
         <v>45677</v>
       </c>
-      <c r="B21" s="4" t="n">
+      <c r="B21" s="5" t="n">
         <v>6</v>
       </c>
       <c r="C21" s="4" t="n">
@@ -742,8 +744,8 @@
       <c r="A22" s="3" t="n">
         <v>45678</v>
       </c>
-      <c r="B22" s="4" t="n">
-        <v>21</v>
+      <c r="B22" s="5" t="n">
+        <v>21.7</v>
       </c>
       <c r="C22" s="4" t="n">
         <v>115</v>
@@ -756,8 +758,8 @@
       <c r="A23" s="3" t="n">
         <v>45679</v>
       </c>
-      <c r="B23" s="4" t="n">
-        <v>12</v>
+      <c r="B23" s="5" t="n">
+        <v>12.6</v>
       </c>
       <c r="C23" s="4" t="n">
         <v>81</v>
@@ -770,8 +772,8 @@
       <c r="A24" s="3" t="n">
         <v>45680</v>
       </c>
-      <c r="B24" s="4" t="n">
-        <v>14</v>
+      <c r="B24" s="5" t="n">
+        <v>14.3</v>
       </c>
       <c r="C24" s="4" t="n">
         <v>128</v>
@@ -784,8 +786,8 @@
       <c r="A25" s="3" t="n">
         <v>45681</v>
       </c>
-      <c r="B25" s="4" t="n">
-        <v>7</v>
+      <c r="B25" s="5" t="n">
+        <v>7.1</v>
       </c>
       <c r="C25" s="4" t="n">
         <v>71</v>
@@ -798,8 +800,8 @@
       <c r="A26" s="3" t="n">
         <v>45682</v>
       </c>
-      <c r="B26" s="4" t="n">
-        <v>12</v>
+      <c r="B26" s="5" t="n">
+        <v>12.9</v>
       </c>
       <c r="C26" s="4" t="n">
         <v>111</v>
@@ -812,8 +814,8 @@
       <c r="A27" s="3" t="n">
         <v>45683</v>
       </c>
-      <c r="B27" s="4" t="n">
-        <v>15</v>
+      <c r="B27" s="5" t="n">
+        <v>15.3</v>
       </c>
       <c r="C27" s="4" t="n">
         <v>143</v>
@@ -826,8 +828,8 @@
       <c r="A28" s="3" t="n">
         <v>45684</v>
       </c>
-      <c r="B28" s="4" t="n">
-        <v>9</v>
+      <c r="B28" s="5" t="n">
+        <v>9.1</v>
       </c>
       <c r="C28" s="4" t="n">
         <v>80</v>
@@ -840,8 +842,8 @@
       <c r="A29" s="3" t="n">
         <v>45685</v>
       </c>
-      <c r="B29" s="4" t="n">
-        <v>17</v>
+      <c r="B29" s="5" t="n">
+        <v>17.1</v>
       </c>
       <c r="C29" s="4" t="n">
         <v>88</v>
@@ -854,8 +856,8 @@
       <c r="A30" s="3" t="n">
         <v>45686</v>
       </c>
-      <c r="B30" s="4" t="n">
-        <v>12</v>
+      <c r="B30" s="5" t="n">
+        <v>12.8</v>
       </c>
       <c r="C30" s="4" t="n">
         <v>101</v>
@@ -868,8 +870,8 @@
       <c r="A31" s="3" t="n">
         <v>45687</v>
       </c>
-      <c r="B31" s="4" t="n">
-        <v>14</v>
+      <c r="B31" s="5" t="n">
+        <v>14.5</v>
       </c>
       <c r="C31" s="4" t="n">
         <v>89</v>
@@ -882,8 +884,8 @@
       <c r="A32" s="3" t="n">
         <v>45688</v>
       </c>
-      <c r="B32" s="4" t="n">
-        <v>13</v>
+      <c r="B32" s="5" t="n">
+        <v>13.7</v>
       </c>
       <c r="C32" s="4" t="n">
         <v>68</v>
@@ -896,8 +898,8 @@
       <c r="A33" s="3" t="n">
         <v>45689</v>
       </c>
-      <c r="B33" s="4" t="n">
-        <v>25</v>
+      <c r="B33" s="5" t="n">
+        <v>25.7</v>
       </c>
       <c r="C33" s="4" t="n">
         <v>101</v>
@@ -910,8 +912,8 @@
       <c r="A34" s="3" t="n">
         <v>45690</v>
       </c>
-      <c r="B34" s="4" t="n">
-        <v>16</v>
+      <c r="B34" s="5" t="n">
+        <v>16.5</v>
       </c>
       <c r="C34" s="4" t="n">
         <v>78</v>
@@ -924,8 +926,8 @@
       <c r="A35" s="3" t="n">
         <v>45691</v>
       </c>
-      <c r="B35" s="4" t="n">
-        <v>11</v>
+      <c r="B35" s="5" t="n">
+        <v>11.9</v>
       </c>
       <c r="C35" s="4" t="n">
         <v>109</v>
@@ -938,8 +940,8 @@
       <c r="A36" s="3" t="n">
         <v>45692</v>
       </c>
-      <c r="B36" s="4" t="n">
-        <v>21</v>
+      <c r="B36" s="5" t="n">
+        <v>21.3</v>
       </c>
       <c r="C36" s="4" t="n">
         <v>81</v>
@@ -952,8 +954,8 @@
       <c r="A37" s="3" t="n">
         <v>45693</v>
       </c>
-      <c r="B37" s="4" t="n">
-        <v>11</v>
+      <c r="B37" s="5" t="n">
+        <v>11.5</v>
       </c>
       <c r="C37" s="4" t="n">
         <v>131</v>
@@ -966,8 +968,8 @@
       <c r="A38" s="3" t="n">
         <v>45694</v>
       </c>
-      <c r="B38" s="4" t="n">
-        <v>19</v>
+      <c r="B38" s="5" t="n">
+        <v>19.7</v>
       </c>
       <c r="C38" s="4" t="n">
         <v>84</v>
@@ -980,8 +982,8 @@
       <c r="A39" s="3" t="n">
         <v>45695</v>
       </c>
-      <c r="B39" s="4" t="n">
-        <v>8</v>
+      <c r="B39" s="5" t="n">
+        <v>8.6</v>
       </c>
       <c r="C39" s="4" t="n">
         <v>93</v>
@@ -994,8 +996,8 @@
       <c r="A40" s="3" t="n">
         <v>45696</v>
       </c>
-      <c r="B40" s="4" t="n">
-        <v>12</v>
+      <c r="B40" s="5" t="n">
+        <v>12.8</v>
       </c>
       <c r="C40" s="4" t="n">
         <v>116</v>
@@ -1008,8 +1010,8 @@
       <c r="A41" s="3" t="n">
         <v>45697</v>
       </c>
-      <c r="B41" s="4" t="n">
-        <v>20</v>
+      <c r="B41" s="5" t="n">
+        <v>20.5</v>
       </c>
       <c r="C41" s="4" t="n">
         <v>75</v>
@@ -1022,8 +1024,8 @@
       <c r="A42" s="3" t="n">
         <v>45698</v>
       </c>
-      <c r="B42" s="4" t="n">
-        <v>23</v>
+      <c r="B42" s="5" t="n">
+        <v>23.6</v>
       </c>
       <c r="C42" s="4" t="n">
         <v>104</v>
@@ -1036,7 +1038,7 @@
       <c r="A43" s="3" t="n">
         <v>45699</v>
       </c>
-      <c r="B43" s="4" t="n">
+      <c r="B43" s="5" t="n">
         <v>20</v>
       </c>
       <c r="C43" s="4" t="n">
@@ -1050,8 +1052,8 @@
       <c r="A44" s="3" t="n">
         <v>45700</v>
       </c>
-      <c r="B44" s="4" t="n">
-        <v>19</v>
+      <c r="B44" s="5" t="n">
+        <v>19.2</v>
       </c>
       <c r="C44" s="4" t="n">
         <v>67</v>
@@ -1064,8 +1066,8 @@
       <c r="A45" s="3" t="n">
         <v>45701</v>
       </c>
-      <c r="B45" s="4" t="n">
-        <v>19</v>
+      <c r="B45" s="5" t="n">
+        <v>19.3</v>
       </c>
       <c r="C45" s="4" t="n">
         <v>103</v>
@@ -1078,8 +1080,8 @@
       <c r="A46" s="3" t="n">
         <v>45702</v>
       </c>
-      <c r="B46" s="4" t="n">
-        <v>13</v>
+      <c r="B46" s="5" t="n">
+        <v>13.1</v>
       </c>
       <c r="C46" s="4" t="n">
         <v>105</v>
@@ -1092,8 +1094,8 @@
       <c r="A47" s="3" t="n">
         <v>45703</v>
       </c>
-      <c r="B47" s="4" t="n">
-        <v>17</v>
+      <c r="B47" s="5" t="n">
+        <v>17.2</v>
       </c>
       <c r="C47" s="4" t="n">
         <v>115</v>
@@ -1106,8 +1108,8 @@
       <c r="A48" s="3" t="n">
         <v>45704</v>
       </c>
-      <c r="B48" s="4" t="n">
-        <v>19</v>
+      <c r="B48" s="5" t="n">
+        <v>19.1</v>
       </c>
       <c r="C48" s="4" t="n">
         <v>75</v>
@@ -1120,8 +1122,8 @@
       <c r="A49" s="3" t="n">
         <v>45705</v>
       </c>
-      <c r="B49" s="4" t="n">
-        <v>27</v>
+      <c r="B49" s="5" t="n">
+        <v>27.3</v>
       </c>
       <c r="C49" s="4" t="n">
         <v>73</v>
@@ -1134,8 +1136,8 @@
       <c r="A50" s="3" t="n">
         <v>45706</v>
       </c>
-      <c r="B50" s="4" t="n">
-        <v>24</v>
+      <c r="B50" s="5" t="n">
+        <v>24.6</v>
       </c>
       <c r="C50" s="4" t="n">
         <v>110</v>
@@ -1148,8 +1150,8 @@
       <c r="A51" s="3" t="n">
         <v>45707</v>
       </c>
-      <c r="B51" s="4" t="n">
-        <v>13</v>
+      <c r="B51" s="5" t="n">
+        <v>13.3</v>
       </c>
       <c r="C51" s="4" t="n">
         <v>105</v>
@@ -1162,8 +1164,8 @@
       <c r="A52" s="3" t="n">
         <v>45708</v>
       </c>
-      <c r="B52" s="4" t="n">
-        <v>24</v>
+      <c r="B52" s="5" t="n">
+        <v>24.3</v>
       </c>
       <c r="C52" s="4" t="n">
         <v>105</v>
@@ -1176,8 +1178,8 @@
       <c r="A53" s="3" t="n">
         <v>45709</v>
       </c>
-      <c r="B53" s="4" t="n">
-        <v>21</v>
+      <c r="B53" s="5" t="n">
+        <v>21.2</v>
       </c>
       <c r="C53" s="4" t="n">
         <v>106</v>
@@ -1190,8 +1192,8 @@
       <c r="A54" s="3" t="n">
         <v>45710</v>
       </c>
-      <c r="B54" s="4" t="n">
-        <v>20</v>
+      <c r="B54" s="5" t="n">
+        <v>20.2</v>
       </c>
       <c r="C54" s="4" t="n">
         <v>86</v>
@@ -1204,8 +1206,8 @@
       <c r="A55" s="3" t="n">
         <v>45711</v>
       </c>
-      <c r="B55" s="4" t="n">
-        <v>27</v>
+      <c r="B55" s="5" t="n">
+        <v>27.8</v>
       </c>
       <c r="C55" s="4" t="n">
         <v>104</v>
@@ -1218,8 +1220,8 @@
       <c r="A56" s="3" t="n">
         <v>45712</v>
       </c>
-      <c r="B56" s="4" t="n">
-        <v>29</v>
+      <c r="B56" s="5" t="n">
+        <v>29.6</v>
       </c>
       <c r="C56" s="4" t="n">
         <v>105</v>
@@ -1232,8 +1234,8 @@
       <c r="A57" s="3" t="n">
         <v>45713</v>
       </c>
-      <c r="B57" s="4" t="n">
-        <v>29</v>
+      <c r="B57" s="5" t="n">
+        <v>29.5</v>
       </c>
       <c r="C57" s="4" t="n">
         <v>85</v>
@@ -1246,8 +1248,8 @@
       <c r="A58" s="3" t="n">
         <v>45714</v>
       </c>
-      <c r="B58" s="4" t="n">
-        <v>21</v>
+      <c r="B58" s="5" t="n">
+        <v>21.2</v>
       </c>
       <c r="C58" s="4" t="n">
         <v>137</v>
@@ -1260,8 +1262,8 @@
       <c r="A59" s="3" t="n">
         <v>45715</v>
       </c>
-      <c r="B59" s="4" t="n">
-        <v>24</v>
+      <c r="B59" s="5" t="n">
+        <v>24.7</v>
       </c>
       <c r="C59" s="4" t="n">
         <v>109</v>
@@ -1274,8 +1276,8 @@
       <c r="A60" s="3" t="n">
         <v>45716</v>
       </c>
-      <c r="B60" s="4" t="n">
-        <v>27</v>
+      <c r="B60" s="5" t="n">
+        <v>27.1</v>
       </c>
       <c r="C60" s="4" t="n">
         <v>76</v>
@@ -1288,8 +1290,8 @@
       <c r="A61" s="3" t="n">
         <v>45717</v>
       </c>
-      <c r="B61" s="4" t="n">
-        <v>31</v>
+      <c r="B61" s="5" t="n">
+        <v>31.3</v>
       </c>
       <c r="C61" s="4" t="n">
         <v>113</v>
@@ -1302,8 +1304,8 @@
       <c r="A62" s="3" t="n">
         <v>45718</v>
       </c>
-      <c r="B62" s="4" t="n">
-        <v>24</v>
+      <c r="B62" s="5" t="n">
+        <v>24.9</v>
       </c>
       <c r="C62" s="4" t="n">
         <v>80</v>
@@ -1316,8 +1318,8 @@
       <c r="A63" s="3" t="n">
         <v>45719</v>
       </c>
-      <c r="B63" s="4" t="n">
-        <v>26</v>
+      <c r="B63" s="5" t="n">
+        <v>26.6</v>
       </c>
       <c r="C63" s="4" t="n">
         <v>115</v>
@@ -1330,8 +1332,8 @@
       <c r="A64" s="3" t="n">
         <v>45720</v>
       </c>
-      <c r="B64" s="4" t="n">
-        <v>22</v>
+      <c r="B64" s="5" t="n">
+        <v>22.5</v>
       </c>
       <c r="C64" s="4" t="n">
         <v>123</v>
@@ -1344,8 +1346,8 @@
       <c r="A65" s="3" t="n">
         <v>45721</v>
       </c>
-      <c r="B65" s="4" t="n">
-        <v>22</v>
+      <c r="B65" s="5" t="n">
+        <v>22.6</v>
       </c>
       <c r="C65" s="4" t="n">
         <v>83</v>
@@ -1358,8 +1360,8 @@
       <c r="A66" s="3" t="n">
         <v>45722</v>
       </c>
-      <c r="B66" s="4" t="n">
-        <v>32</v>
+      <c r="B66" s="5" t="n">
+        <v>32.8</v>
       </c>
       <c r="C66" s="4" t="n">
         <v>119</v>
@@ -1372,8 +1374,8 @@
       <c r="A67" s="3" t="n">
         <v>45723</v>
       </c>
-      <c r="B67" s="4" t="n">
-        <v>35</v>
+      <c r="B67" s="5" t="n">
+        <v>35.7</v>
       </c>
       <c r="C67" s="4" t="n">
         <v>108</v>
@@ -1386,8 +1388,8 @@
       <c r="A68" s="3" t="n">
         <v>45724</v>
       </c>
-      <c r="B68" s="4" t="n">
-        <v>29</v>
+      <c r="B68" s="5" t="n">
+        <v>29.2</v>
       </c>
       <c r="C68" s="4" t="n">
         <v>116</v>
@@ -1400,7 +1402,7 @@
       <c r="A69" s="3" t="n">
         <v>45725</v>
       </c>
-      <c r="B69" s="4" t="n">
+      <c r="B69" s="5" t="n">
         <v>34</v>
       </c>
       <c r="C69" s="4" t="n">
@@ -1414,8 +1416,8 @@
       <c r="A70" s="3" t="n">
         <v>45726</v>
       </c>
-      <c r="B70" s="4" t="n">
-        <v>32</v>
+      <c r="B70" s="5" t="n">
+        <v>32.3</v>
       </c>
       <c r="C70" s="4" t="n">
         <v>95</v>
@@ -1428,8 +1430,8 @@
       <c r="A71" s="3" t="n">
         <v>45727</v>
       </c>
-      <c r="B71" s="4" t="n">
-        <v>27</v>
+      <c r="B71" s="5" t="n">
+        <v>27.2</v>
       </c>
       <c r="C71" s="4" t="n">
         <v>84</v>
@@ -1442,8 +1444,8 @@
       <c r="A72" s="3" t="n">
         <v>45728</v>
       </c>
-      <c r="B72" s="4" t="n">
-        <v>32</v>
+      <c r="B72" s="5" t="n">
+        <v>32.2</v>
       </c>
       <c r="C72" s="4" t="n">
         <v>82</v>
@@ -1456,8 +1458,8 @@
       <c r="A73" s="3" t="n">
         <v>45729</v>
       </c>
-      <c r="B73" s="4" t="n">
-        <v>39</v>
+      <c r="B73" s="5" t="n">
+        <v>39.8</v>
       </c>
       <c r="C73" s="4" t="n">
         <v>83</v>
@@ -1470,8 +1472,8 @@
       <c r="A74" s="3" t="n">
         <v>45730</v>
       </c>
-      <c r="B74" s="4" t="n">
-        <v>31</v>
+      <c r="B74" s="5" t="n">
+        <v>31.8</v>
       </c>
       <c r="C74" s="4" t="n">
         <v>98</v>
@@ -1484,8 +1486,8 @@
       <c r="A75" s="3" t="n">
         <v>45731</v>
       </c>
-      <c r="B75" s="4" t="n">
-        <v>40</v>
+      <c r="B75" s="5" t="n">
+        <v>40.3</v>
       </c>
       <c r="C75" s="4" t="n">
         <v>106</v>
@@ -1498,8 +1500,8 @@
       <c r="A76" s="3" t="n">
         <v>45732</v>
       </c>
-      <c r="B76" s="4" t="n">
-        <v>19</v>
+      <c r="B76" s="5" t="n">
+        <v>19.6</v>
       </c>
       <c r="C76" s="4" t="n">
         <v>105</v>
@@ -1512,8 +1514,8 @@
       <c r="A77" s="3" t="n">
         <v>45733</v>
       </c>
-      <c r="B77" s="4" t="n">
-        <v>37</v>
+      <c r="B77" s="5" t="n">
+        <v>37.4</v>
       </c>
       <c r="C77" s="4" t="n">
         <v>116</v>
@@ -1526,8 +1528,8 @@
       <c r="A78" s="3" t="n">
         <v>45734</v>
       </c>
-      <c r="B78" s="4" t="n">
-        <v>34</v>
+      <c r="B78" s="5" t="n">
+        <v>34.8</v>
       </c>
       <c r="C78" s="4" t="n">
         <v>100</v>
@@ -1540,8 +1542,8 @@
       <c r="A79" s="3" t="n">
         <v>45735</v>
       </c>
-      <c r="B79" s="4" t="n">
-        <v>32</v>
+      <c r="B79" s="5" t="n">
+        <v>32.4</v>
       </c>
       <c r="C79" s="4" t="n">
         <v>129</v>
@@ -1554,8 +1556,8 @@
       <c r="A80" s="3" t="n">
         <v>45736</v>
       </c>
-      <c r="B80" s="4" t="n">
-        <v>35</v>
+      <c r="B80" s="5" t="n">
+        <v>35.2</v>
       </c>
       <c r="C80" s="4" t="n">
         <v>94</v>
@@ -1568,8 +1570,8 @@
       <c r="A81" s="3" t="n">
         <v>45737</v>
       </c>
-      <c r="B81" s="4" t="n">
-        <v>25</v>
+      <c r="B81" s="5" t="n">
+        <v>25.2</v>
       </c>
       <c r="C81" s="4" t="n">
         <v>154</v>
@@ -1582,8 +1584,8 @@
       <c r="A82" s="3" t="n">
         <v>45738</v>
       </c>
-      <c r="B82" s="4" t="n">
-        <v>34</v>
+      <c r="B82" s="5" t="n">
+        <v>34.5</v>
       </c>
       <c r="C82" s="4" t="n">
         <v>112</v>
@@ -1596,8 +1598,8 @@
       <c r="A83" s="3" t="n">
         <v>45739</v>
       </c>
-      <c r="B83" s="4" t="n">
-        <v>37</v>
+      <c r="B83" s="5" t="n">
+        <v>37.2</v>
       </c>
       <c r="C83" s="4" t="n">
         <v>82</v>
@@ -1610,8 +1612,8 @@
       <c r="A84" s="3" t="n">
         <v>45740</v>
       </c>
-      <c r="B84" s="4" t="n">
-        <v>43</v>
+      <c r="B84" s="5" t="n">
+        <v>43.5</v>
       </c>
       <c r="C84" s="4" t="n">
         <v>78</v>
@@ -1624,8 +1626,8 @@
       <c r="A85" s="3" t="n">
         <v>45741</v>
       </c>
-      <c r="B85" s="4" t="n">
-        <v>34</v>
+      <c r="B85" s="5" t="n">
+        <v>34.8</v>
       </c>
       <c r="C85" s="4" t="n">
         <v>109</v>
@@ -1638,8 +1640,8 @@
       <c r="A86" s="3" t="n">
         <v>45742</v>
       </c>
-      <c r="B86" s="4" t="n">
-        <v>33</v>
+      <c r="B86" s="5" t="n">
+        <v>33.4</v>
       </c>
       <c r="C86" s="4" t="n">
         <v>95</v>
@@ -1652,8 +1654,8 @@
       <c r="A87" s="3" t="n">
         <v>45743</v>
       </c>
-      <c r="B87" s="4" t="n">
-        <v>35</v>
+      <c r="B87" s="5" t="n">
+        <v>35.2</v>
       </c>
       <c r="C87" s="4" t="n">
         <v>114</v>
@@ -1666,8 +1668,8 @@
       <c r="A88" s="3" t="n">
         <v>45744</v>
       </c>
-      <c r="B88" s="4" t="n">
-        <v>42</v>
+      <c r="B88" s="5" t="n">
+        <v>42.9</v>
       </c>
       <c r="C88" s="4" t="n">
         <v>109</v>
@@ -1680,8 +1682,8 @@
       <c r="A89" s="3" t="n">
         <v>45745</v>
       </c>
-      <c r="B89" s="4" t="n">
-        <v>40</v>
+      <c r="B89" s="5" t="n">
+        <v>40.5</v>
       </c>
       <c r="C89" s="4" t="n">
         <v>98</v>
@@ -1694,8 +1696,8 @@
       <c r="A90" s="3" t="n">
         <v>45746</v>
       </c>
-      <c r="B90" s="4" t="n">
-        <v>36</v>
+      <c r="B90" s="5" t="n">
+        <v>36.1</v>
       </c>
       <c r="C90" s="4" t="n">
         <v>83</v>
@@ -1708,7 +1710,7 @@
       <c r="A91" s="3" t="n">
         <v>45747</v>
       </c>
-      <c r="B91" s="4" t="n">
+      <c r="B91" s="5" t="n">
         <v>41</v>
       </c>
       <c r="C91" s="4" t="n">
@@ -1722,8 +1724,8 @@
       <c r="A92" s="3" t="n">
         <v>45748</v>
       </c>
-      <c r="B92" s="4" t="n">
-        <v>40</v>
+      <c r="B92" s="5" t="n">
+        <v>40.1</v>
       </c>
       <c r="C92" s="4" t="n">
         <v>91</v>
@@ -1736,8 +1738,8 @@
       <c r="A93" s="3" t="n">
         <v>45749</v>
       </c>
-      <c r="B93" s="4" t="n">
-        <v>45</v>
+      <c r="B93" s="5" t="n">
+        <v>45.6</v>
       </c>
       <c r="C93" s="4" t="n">
         <v>117</v>
@@ -1750,8 +1752,8 @@
       <c r="A94" s="3" t="n">
         <v>45750</v>
       </c>
-      <c r="B94" s="4" t="n">
-        <v>37</v>
+      <c r="B94" s="5" t="n">
+        <v>37.7</v>
       </c>
       <c r="C94" s="4" t="n">
         <v>104</v>
@@ -1764,8 +1766,8 @@
       <c r="A95" s="3" t="n">
         <v>45751</v>
       </c>
-      <c r="B95" s="4" t="n">
-        <v>39</v>
+      <c r="B95" s="5" t="n">
+        <v>39.4</v>
       </c>
       <c r="C95" s="4" t="n">
         <v>75</v>
@@ -1778,8 +1780,8 @@
       <c r="A96" s="3" t="n">
         <v>45752</v>
       </c>
-      <c r="B96" s="4" t="n">
-        <v>39</v>
+      <c r="B96" s="5" t="n">
+        <v>39.1</v>
       </c>
       <c r="C96" s="4" t="n">
         <v>103</v>
@@ -1792,8 +1794,8 @@
       <c r="A97" s="3" t="n">
         <v>45753</v>
       </c>
-      <c r="B97" s="4" t="n">
-        <v>34</v>
+      <c r="B97" s="5" t="n">
+        <v>34.3</v>
       </c>
       <c r="C97" s="4" t="n">
         <v>107</v>
@@ -1806,8 +1808,8 @@
       <c r="A98" s="3" t="n">
         <v>45754</v>
       </c>
-      <c r="B98" s="4" t="n">
-        <v>43</v>
+      <c r="B98" s="5" t="n">
+        <v>43.9</v>
       </c>
       <c r="C98" s="4" t="n">
         <v>82</v>
@@ -1820,8 +1822,8 @@
       <c r="A99" s="3" t="n">
         <v>45755</v>
       </c>
-      <c r="B99" s="4" t="n">
-        <v>43</v>
+      <c r="B99" s="5" t="n">
+        <v>43.5</v>
       </c>
       <c r="C99" s="4" t="n">
         <v>103</v>
@@ -1834,8 +1836,8 @@
       <c r="A100" s="3" t="n">
         <v>45756</v>
       </c>
-      <c r="B100" s="4" t="n">
-        <v>43</v>
+      <c r="B100" s="5" t="n">
+        <v>43.9</v>
       </c>
       <c r="C100" s="4" t="n">
         <v>101</v>
@@ -1848,8 +1850,8 @@
       <c r="A101" s="3" t="n">
         <v>45757</v>
       </c>
-      <c r="B101" s="4" t="n">
-        <v>42</v>
+      <c r="B101" s="5" t="n">
+        <v>42.8</v>
       </c>
       <c r="C101" s="4" t="n">
         <v>77</v>

</xml_diff>